<commit_message>
Final commit before day/night tile swap optimization. Only comment changes as far as I know.
</commit_message>
<xml_diff>
--- a/Map_Shapes/Map/() darkness/TOD, ELS, PLS Charts v0.01.xlsx
+++ b/Map_Shapes/Map/() darkness/TOD, ELS, PLS Charts v0.01.xlsx
@@ -2504,7 +2504,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2532,6 +2532,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2614,7 +2620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -2670,6 +2676,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -19779,8 +19788,8 @@
   </sheetPr>
   <dimension ref="A1:BS240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z214" sqref="Z214"/>
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C173" sqref="C173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19789,7 +19798,7 @@
     <col min="2" max="2" width="42" customWidth="1"/>
     <col min="3" max="3" width="5.28515625" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" customWidth="1"/>
+    <col min="6" max="10" width="9.140625" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
     <col min="72" max="72" width="9" customWidth="1"/>
   </cols>
@@ -27139,95 +27148,95 @@
         <v>0</v>
       </c>
       <c r="F177" s="33"/>
-      <c r="G177" s="34" t="str">
+      <c r="G177" s="35" t="str">
         <f>DEC2HEX(G223)</f>
         <v>0</v>
       </c>
-      <c r="H177" s="34" t="str">
+      <c r="H177" s="35" t="str">
         <f t="shared" ref="H177:AC177" si="14">DEC2HEX(H223)</f>
         <v>1</v>
       </c>
-      <c r="I177" s="34" t="str">
+      <c r="I177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="J177" s="34" t="str">
+      <c r="J177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>3</v>
       </c>
-      <c r="K177" s="34" t="str">
+      <c r="K177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="L177" s="34" t="str">
+      <c r="L177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>5</v>
       </c>
-      <c r="M177" s="34" t="str">
+      <c r="M177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>6</v>
       </c>
-      <c r="N177" s="34" t="str">
+      <c r="N177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>7</v>
       </c>
-      <c r="O177" s="34" t="str">
+      <c r="O177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>8</v>
       </c>
-      <c r="P177" s="34" t="str">
+      <c r="P177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>9</v>
       </c>
-      <c r="Q177" s="34" t="str">
+      <c r="Q177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>A</v>
       </c>
-      <c r="R177" s="34" t="str">
+      <c r="R177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>B</v>
       </c>
-      <c r="S177" s="34" t="str">
+      <c r="S177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>C</v>
       </c>
-      <c r="T177" s="34" t="str">
+      <c r="T177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>D</v>
       </c>
-      <c r="U177" s="34" t="str">
+      <c r="U177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>E</v>
       </c>
-      <c r="V177" s="34" t="str">
+      <c r="V177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>F</v>
       </c>
-      <c r="W177" s="34" t="str">
+      <c r="W177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>10</v>
       </c>
-      <c r="X177" s="34" t="str">
+      <c r="X177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>11</v>
       </c>
-      <c r="Y177" s="34" t="str">
+      <c r="Y177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>12</v>
       </c>
-      <c r="Z177" s="34" t="str">
+      <c r="Z177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>13</v>
       </c>
-      <c r="AA177" s="34" t="str">
+      <c r="AA177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>14</v>
       </c>
-      <c r="AB177" s="34" t="str">
+      <c r="AB177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>15</v>
       </c>
-      <c r="AC177" s="34" t="str">
+      <c r="AC177" s="35" t="str">
         <f t="shared" si="14"/>
         <v>16</v>
       </c>
@@ -27238,95 +27247,95 @@
       </c>
       <c r="E178" s="33"/>
       <c r="F178" s="33"/>
-      <c r="G178" s="34" t="str">
+      <c r="G178" s="35" t="str">
         <f t="shared" ref="G178:AC178" si="15">DEC2HEX(G224)</f>
         <v>17</v>
       </c>
-      <c r="H178" s="34" t="str">
+      <c r="H178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>18</v>
       </c>
-      <c r="I178" s="34" t="str">
+      <c r="I178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>19</v>
       </c>
-      <c r="J178" s="34" t="str">
+      <c r="J178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>1A</v>
       </c>
-      <c r="K178" s="34" t="str">
+      <c r="K178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>1B</v>
       </c>
-      <c r="L178" s="34" t="str">
+      <c r="L178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>1C</v>
       </c>
-      <c r="M178" s="34" t="str">
+      <c r="M178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>1D</v>
       </c>
-      <c r="N178" s="34" t="str">
+      <c r="N178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>1E</v>
       </c>
-      <c r="O178" s="34" t="str">
+      <c r="O178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>1F</v>
       </c>
-      <c r="P178" s="34" t="str">
+      <c r="P178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>20</v>
       </c>
-      <c r="Q178" s="34" t="str">
+      <c r="Q178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>21</v>
       </c>
-      <c r="R178" s="34" t="str">
+      <c r="R178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>22</v>
       </c>
-      <c r="S178" s="34" t="str">
+      <c r="S178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>23</v>
       </c>
-      <c r="T178" s="34" t="str">
+      <c r="T178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>24</v>
       </c>
-      <c r="U178" s="34" t="str">
+      <c r="U178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>25</v>
       </c>
-      <c r="V178" s="34" t="str">
+      <c r="V178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>26</v>
       </c>
-      <c r="W178" s="34" t="str">
+      <c r="W178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>27</v>
       </c>
-      <c r="X178" s="34" t="str">
+      <c r="X178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>28</v>
       </c>
-      <c r="Y178" s="34" t="str">
+      <c r="Y178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>29</v>
       </c>
-      <c r="Z178" s="34" t="str">
+      <c r="Z178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>2A</v>
       </c>
-      <c r="AA178" s="34" t="str">
+      <c r="AA178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>2B</v>
       </c>
-      <c r="AB178" s="34" t="str">
+      <c r="AB178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>2C</v>
       </c>
-      <c r="AC178" s="34" t="str">
+      <c r="AC178" s="35" t="str">
         <f t="shared" si="15"/>
         <v>2D</v>
       </c>
@@ -27337,95 +27346,95 @@
       </c>
       <c r="E179" s="33"/>
       <c r="F179" s="33"/>
-      <c r="G179" s="34" t="str">
+      <c r="G179" s="35" t="str">
         <f t="shared" ref="G179:AC179" si="16">DEC2HEX(G225)</f>
         <v>2E</v>
       </c>
-      <c r="H179" s="34" t="str">
+      <c r="H179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>2F</v>
       </c>
-      <c r="I179" s="34" t="str">
+      <c r="I179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>30</v>
       </c>
-      <c r="J179" s="34" t="str">
+      <c r="J179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>31</v>
       </c>
-      <c r="K179" s="34" t="str">
+      <c r="K179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>32</v>
       </c>
-      <c r="L179" s="34" t="str">
+      <c r="L179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>33</v>
       </c>
-      <c r="M179" s="34" t="str">
+      <c r="M179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>34</v>
       </c>
-      <c r="N179" s="34" t="str">
+      <c r="N179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>35</v>
       </c>
-      <c r="O179" s="34" t="str">
+      <c r="O179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>36</v>
       </c>
-      <c r="P179" s="34" t="str">
+      <c r="P179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>37</v>
       </c>
-      <c r="Q179" s="34" t="str">
+      <c r="Q179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>38</v>
       </c>
-      <c r="R179" s="34" t="str">
+      <c r="R179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>39</v>
       </c>
-      <c r="S179" s="34" t="str">
+      <c r="S179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>3A</v>
       </c>
-      <c r="T179" s="34" t="str">
+      <c r="T179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>3B</v>
       </c>
-      <c r="U179" s="34" t="str">
+      <c r="U179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>3C</v>
       </c>
-      <c r="V179" s="34" t="str">
+      <c r="V179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>3D</v>
       </c>
-      <c r="W179" s="34" t="str">
+      <c r="W179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>3E</v>
       </c>
-      <c r="X179" s="34" t="str">
+      <c r="X179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>3F</v>
       </c>
-      <c r="Y179" s="34" t="str">
+      <c r="Y179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>40</v>
       </c>
-      <c r="Z179" s="34" t="str">
+      <c r="Z179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>41</v>
       </c>
-      <c r="AA179" s="34" t="str">
+      <c r="AA179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>42</v>
       </c>
-      <c r="AB179" s="34" t="str">
+      <c r="AB179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>43</v>
       </c>
-      <c r="AC179" s="34" t="str">
+      <c r="AC179" s="35" t="str">
         <f t="shared" si="16"/>
         <v>44</v>
       </c>
@@ -27436,95 +27445,95 @@
       </c>
       <c r="E180" s="33"/>
       <c r="F180" s="33"/>
-      <c r="G180" s="34" t="str">
+      <c r="G180" s="35" t="str">
         <f t="shared" ref="G180:AC180" si="17">DEC2HEX(G226)</f>
         <v>45</v>
       </c>
-      <c r="H180" s="34" t="str">
+      <c r="H180" s="35" t="str">
         <f t="shared" si="17"/>
         <v>46</v>
       </c>
-      <c r="I180" s="34" t="str">
+      <c r="I180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>47</v>
       </c>
-      <c r="J180" s="34" t="str">
+      <c r="J180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>48</v>
       </c>
-      <c r="K180" s="34" t="str">
+      <c r="K180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>49</v>
       </c>
-      <c r="L180" s="34" t="str">
+      <c r="L180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>4A</v>
       </c>
-      <c r="M180" s="34" t="str">
+      <c r="M180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>4B</v>
       </c>
-      <c r="N180" s="34" t="str">
+      <c r="N180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>4C</v>
       </c>
-      <c r="O180" s="34" t="str">
+      <c r="O180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>4D</v>
       </c>
-      <c r="P180" s="34" t="str">
+      <c r="P180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>4E</v>
       </c>
-      <c r="Q180" s="34" t="str">
+      <c r="Q180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>4F</v>
       </c>
-      <c r="R180" s="34" t="str">
+      <c r="R180" s="28" t="str">
         <f t="shared" si="17"/>
         <v>50</v>
       </c>
-      <c r="S180" s="34" t="str">
+      <c r="S180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>51</v>
       </c>
-      <c r="T180" s="34" t="str">
+      <c r="T180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>52</v>
       </c>
-      <c r="U180" s="34" t="str">
+      <c r="U180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>53</v>
       </c>
-      <c r="V180" s="34" t="str">
+      <c r="V180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>54</v>
       </c>
-      <c r="W180" s="34" t="str">
+      <c r="W180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>55</v>
       </c>
-      <c r="X180" s="34" t="str">
+      <c r="X180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>56</v>
       </c>
-      <c r="Y180" s="34" t="str">
+      <c r="Y180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>57</v>
       </c>
-      <c r="Z180" s="34" t="str">
+      <c r="Z180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>58</v>
       </c>
-      <c r="AA180" s="34" t="str">
+      <c r="AA180" s="23" t="str">
         <f t="shared" si="17"/>
         <v>59</v>
       </c>
-      <c r="AB180" s="34" t="str">
+      <c r="AB180" s="35" t="str">
         <f t="shared" si="17"/>
         <v>5A</v>
       </c>
-      <c r="AC180" s="34" t="str">
+      <c r="AC180" s="35" t="str">
         <f t="shared" si="17"/>
         <v>5B</v>
       </c>
@@ -27540,95 +27549,95 @@
         <v>38</v>
       </c>
       <c r="F181" s="4"/>
-      <c r="G181" s="34" t="str">
+      <c r="G181" s="35" t="str">
         <f t="shared" ref="G181:AC181" si="18">DEC2HEX(G227)</f>
         <v>5C</v>
       </c>
-      <c r="H181" s="34" t="str">
+      <c r="H181" s="35" t="str">
         <f t="shared" si="18"/>
         <v>5D</v>
       </c>
-      <c r="I181" s="34" t="str">
+      <c r="I181" s="23" t="str">
         <f t="shared" si="18"/>
         <v>5E</v>
       </c>
-      <c r="J181" s="34" t="str">
+      <c r="J181" s="23" t="str">
         <f t="shared" si="18"/>
         <v>5F</v>
       </c>
-      <c r="K181" s="34" t="str">
+      <c r="K181" s="23" t="str">
         <f t="shared" si="18"/>
         <v>60</v>
       </c>
-      <c r="L181" s="34" t="str">
+      <c r="L181" s="23" t="str">
         <f t="shared" si="18"/>
         <v>61</v>
       </c>
-      <c r="M181" s="34" t="str">
+      <c r="M181" s="23" t="str">
         <f t="shared" si="18"/>
         <v>62</v>
       </c>
-      <c r="N181" s="34" t="str">
+      <c r="N181" s="23" t="str">
         <f t="shared" si="18"/>
         <v>63</v>
       </c>
-      <c r="O181" s="34" t="str">
+      <c r="O181" s="24" t="str">
         <f t="shared" si="18"/>
         <v>64</v>
       </c>
-      <c r="P181" s="34" t="str">
+      <c r="P181" s="24" t="str">
         <f t="shared" si="18"/>
         <v>65</v>
       </c>
-      <c r="Q181" s="34" t="str">
+      <c r="Q181" s="24" t="str">
         <f t="shared" si="18"/>
         <v>66</v>
       </c>
-      <c r="R181" s="34" t="str">
+      <c r="R181" s="24" t="str">
         <f t="shared" si="18"/>
         <v>67</v>
       </c>
-      <c r="S181" s="34" t="str">
+      <c r="S181" s="24" t="str">
         <f t="shared" si="18"/>
         <v>68</v>
       </c>
-      <c r="T181" s="34" t="str">
+      <c r="T181" s="24" t="str">
         <f t="shared" si="18"/>
         <v>69</v>
       </c>
-      <c r="U181" s="34" t="str">
+      <c r="U181" s="24" t="str">
         <f t="shared" si="18"/>
         <v>6A</v>
       </c>
-      <c r="V181" s="34" t="str">
+      <c r="V181" s="23" t="str">
         <f t="shared" si="18"/>
         <v>6B</v>
       </c>
-      <c r="W181" s="34" t="str">
+      <c r="W181" s="23" t="str">
         <f t="shared" si="18"/>
         <v>6C</v>
       </c>
-      <c r="X181" s="34" t="str">
+      <c r="X181" s="23" t="str">
         <f t="shared" si="18"/>
         <v>6D</v>
       </c>
-      <c r="Y181" s="34" t="str">
+      <c r="Y181" s="23" t="str">
         <f t="shared" si="18"/>
         <v>6E</v>
       </c>
-      <c r="Z181" s="34" t="str">
+      <c r="Z181" s="23" t="str">
         <f t="shared" si="18"/>
         <v>6F</v>
       </c>
-      <c r="AA181" s="34" t="str">
+      <c r="AA181" s="23" t="str">
         <f t="shared" si="18"/>
         <v>70</v>
       </c>
-      <c r="AB181" s="34" t="str">
+      <c r="AB181" s="35" t="str">
         <f t="shared" si="18"/>
         <v>71</v>
       </c>
-      <c r="AC181" s="34" t="str">
+      <c r="AC181" s="35" t="str">
         <f t="shared" si="18"/>
         <v>72</v>
       </c>
@@ -27644,95 +27653,95 @@
         <v>39</v>
       </c>
       <c r="F182" s="4"/>
-      <c r="G182" s="34" t="str">
+      <c r="G182" s="35" t="str">
         <f t="shared" ref="G182:AC182" si="19">DEC2HEX(G228)</f>
         <v>73</v>
       </c>
-      <c r="H182" s="34" t="str">
+      <c r="H182" s="35" t="str">
         <f t="shared" si="19"/>
         <v>74</v>
       </c>
-      <c r="I182" s="34" t="str">
+      <c r="I182" s="23" t="str">
         <f t="shared" si="19"/>
         <v>75</v>
       </c>
-      <c r="J182" s="34" t="str">
+      <c r="J182" s="23" t="str">
         <f t="shared" si="19"/>
         <v>76</v>
       </c>
-      <c r="K182" s="34" t="str">
+      <c r="K182" s="23" t="str">
         <f t="shared" si="19"/>
         <v>77</v>
       </c>
-      <c r="L182" s="34" t="str">
+      <c r="L182" s="23" t="str">
         <f t="shared" si="19"/>
         <v>78</v>
       </c>
-      <c r="M182" s="34" t="str">
+      <c r="M182" s="23" t="str">
         <f t="shared" si="19"/>
         <v>79</v>
       </c>
-      <c r="N182" s="34" t="str">
+      <c r="N182" s="23" t="str">
         <f t="shared" si="19"/>
         <v>7A</v>
       </c>
-      <c r="O182" s="34" t="str">
+      <c r="O182" s="29" t="str">
         <f t="shared" si="19"/>
         <v>7B</v>
       </c>
-      <c r="P182" s="34" t="str">
+      <c r="P182" s="24" t="str">
         <f t="shared" si="19"/>
         <v>7C</v>
       </c>
-      <c r="Q182" s="34" t="str">
+      <c r="Q182" s="25" t="str">
         <f t="shared" si="19"/>
         <v>7D</v>
       </c>
-      <c r="R182" s="34" t="str">
+      <c r="R182" s="24" t="str">
         <f t="shared" si="19"/>
         <v>7E</v>
       </c>
-      <c r="S182" s="34" t="str">
+      <c r="S182" s="25" t="str">
         <f t="shared" si="19"/>
         <v>7F</v>
       </c>
-      <c r="T182" s="34" t="str">
+      <c r="T182" s="24" t="str">
         <f t="shared" si="19"/>
         <v>80</v>
       </c>
-      <c r="U182" s="34" t="str">
+      <c r="U182" s="29" t="str">
         <f t="shared" si="19"/>
         <v>81</v>
       </c>
-      <c r="V182" s="34" t="str">
+      <c r="V182" s="23" t="str">
         <f t="shared" si="19"/>
         <v>82</v>
       </c>
-      <c r="W182" s="34" t="str">
+      <c r="W182" s="23" t="str">
         <f t="shared" si="19"/>
         <v>83</v>
       </c>
-      <c r="X182" s="34" t="str">
+      <c r="X182" s="23" t="str">
         <f t="shared" si="19"/>
         <v>84</v>
       </c>
-      <c r="Y182" s="34" t="str">
+      <c r="Y182" s="23" t="str">
         <f t="shared" si="19"/>
         <v>85</v>
       </c>
-      <c r="Z182" s="34" t="str">
+      <c r="Z182" s="23" t="str">
         <f t="shared" si="19"/>
         <v>86</v>
       </c>
-      <c r="AA182" s="34" t="str">
+      <c r="AA182" s="23" t="str">
         <f t="shared" si="19"/>
         <v>87</v>
       </c>
-      <c r="AB182" s="34" t="str">
+      <c r="AB182" s="35" t="str">
         <f t="shared" si="19"/>
         <v>88</v>
       </c>
-      <c r="AC182" s="34" t="str">
+      <c r="AC182" s="35" t="str">
         <f t="shared" si="19"/>
         <v>89</v>
       </c>
@@ -27748,95 +27757,95 @@
         <v>40</v>
       </c>
       <c r="F183" s="4"/>
-      <c r="G183" s="34" t="str">
+      <c r="G183" s="35" t="str">
         <f t="shared" ref="G183:AC183" si="20">DEC2HEX(G229)</f>
         <v>8A</v>
       </c>
-      <c r="H183" s="34" t="str">
+      <c r="H183" s="35" t="str">
         <f t="shared" si="20"/>
         <v>8B</v>
       </c>
-      <c r="I183" s="34" t="str">
+      <c r="I183" s="23" t="str">
         <f t="shared" si="20"/>
         <v>8C</v>
       </c>
-      <c r="J183" s="34" t="str">
+      <c r="J183" s="24" t="str">
         <f t="shared" si="20"/>
         <v>8D</v>
       </c>
-      <c r="K183" s="34" t="str">
+      <c r="K183" s="29" t="str">
         <f t="shared" si="20"/>
         <v>8E</v>
       </c>
-      <c r="L183" s="34" t="str">
+      <c r="L183" s="29" t="str">
         <f t="shared" si="20"/>
         <v>8F</v>
       </c>
-      <c r="M183" s="34" t="str">
+      <c r="M183" s="23" t="str">
         <f t="shared" si="20"/>
         <v>90</v>
       </c>
-      <c r="N183" s="34" t="str">
+      <c r="N183" s="23" t="str">
         <f t="shared" si="20"/>
         <v>91</v>
       </c>
-      <c r="O183" s="34" t="str">
+      <c r="O183" s="29" t="str">
         <f t="shared" si="20"/>
         <v>92</v>
       </c>
-      <c r="P183" s="34" t="str">
+      <c r="P183" s="29" t="str">
         <f t="shared" si="20"/>
         <v>93</v>
       </c>
-      <c r="Q183" s="34" t="str">
+      <c r="Q183" s="24" t="str">
         <f t="shared" si="20"/>
         <v>94</v>
       </c>
-      <c r="R183" s="34" t="str">
+      <c r="R183" s="24" t="str">
         <f t="shared" si="20"/>
         <v>95</v>
       </c>
-      <c r="S183" s="34" t="str">
+      <c r="S183" s="24" t="str">
         <f t="shared" si="20"/>
         <v>96</v>
       </c>
-      <c r="T183" s="34" t="str">
+      <c r="T183" s="29" t="str">
         <f t="shared" si="20"/>
         <v>97</v>
       </c>
-      <c r="U183" s="34" t="str">
+      <c r="U183" s="29" t="str">
         <f t="shared" si="20"/>
         <v>98</v>
       </c>
-      <c r="V183" s="34" t="str">
+      <c r="V183" s="23" t="str">
         <f t="shared" si="20"/>
         <v>99</v>
       </c>
-      <c r="W183" s="34" t="str">
+      <c r="W183" s="23" t="str">
         <f t="shared" si="20"/>
         <v>9A</v>
       </c>
-      <c r="X183" s="34" t="str">
+      <c r="X183" s="23" t="str">
         <f t="shared" si="20"/>
         <v>9B</v>
       </c>
-      <c r="Y183" s="34" t="str">
+      <c r="Y183" s="23" t="str">
         <f t="shared" si="20"/>
         <v>9C</v>
       </c>
-      <c r="Z183" s="34" t="str">
+      <c r="Z183" s="24" t="str">
         <f t="shared" si="20"/>
         <v>9D</v>
       </c>
-      <c r="AA183" s="34" t="str">
+      <c r="AA183" s="23" t="str">
         <f t="shared" si="20"/>
         <v>9E</v>
       </c>
-      <c r="AB183" s="34" t="str">
+      <c r="AB183" s="35" t="str">
         <f t="shared" si="20"/>
         <v>9F</v>
       </c>
-      <c r="AC183" s="34" t="str">
+      <c r="AC183" s="35" t="str">
         <f t="shared" si="20"/>
         <v>A0</v>
       </c>
@@ -27852,95 +27861,95 @@
         <v>41</v>
       </c>
       <c r="F184" s="4"/>
-      <c r="G184" s="34" t="str">
+      <c r="G184" s="35" t="str">
         <f t="shared" ref="G184:AC184" si="21">DEC2HEX(G230)</f>
         <v>A1</v>
       </c>
-      <c r="H184" s="34" t="str">
+      <c r="H184" s="35" t="str">
         <f t="shared" si="21"/>
         <v>A2</v>
       </c>
-      <c r="I184" s="34" t="str">
+      <c r="I184" s="23" t="str">
         <f t="shared" si="21"/>
         <v>A3</v>
       </c>
-      <c r="J184" s="34" t="str">
+      <c r="J184" s="25" t="str">
         <f t="shared" si="21"/>
         <v>A4</v>
       </c>
-      <c r="K184" s="34" t="str">
+      <c r="K184" s="24" t="str">
         <f t="shared" si="21"/>
         <v>A5</v>
       </c>
-      <c r="L184" s="34" t="str">
+      <c r="L184" s="29" t="str">
         <f t="shared" si="21"/>
         <v>A6</v>
       </c>
-      <c r="M184" s="34" t="str">
+      <c r="M184" s="23" t="str">
         <f t="shared" si="21"/>
         <v>A7</v>
       </c>
-      <c r="N184" s="34" t="str">
+      <c r="N184" s="23" t="str">
         <f t="shared" si="21"/>
         <v>A8</v>
       </c>
-      <c r="O184" s="34" t="str">
+      <c r="O184" s="23" t="str">
         <f t="shared" si="21"/>
         <v>A9</v>
       </c>
-      <c r="P184" s="34" t="str">
+      <c r="P184" s="23" t="str">
         <f t="shared" si="21"/>
         <v>AA</v>
       </c>
-      <c r="Q184" s="34" t="str">
+      <c r="Q184" s="23" t="str">
         <f t="shared" si="21"/>
         <v>AB</v>
       </c>
-      <c r="R184" s="34" t="str">
+      <c r="R184" s="23" t="str">
         <f t="shared" si="21"/>
         <v>AC</v>
       </c>
-      <c r="S184" s="34" t="str">
+      <c r="S184" s="23" t="str">
         <f t="shared" si="21"/>
         <v>AD</v>
       </c>
-      <c r="T184" s="34" t="str">
+      <c r="T184" s="23" t="str">
         <f t="shared" si="21"/>
         <v>AE</v>
       </c>
-      <c r="U184" s="34" t="str">
+      <c r="U184" s="23" t="str">
         <f t="shared" si="21"/>
         <v>AF</v>
       </c>
-      <c r="V184" s="34" t="str">
+      <c r="V184" s="23" t="str">
         <f t="shared" si="21"/>
         <v>B0</v>
       </c>
-      <c r="W184" s="34" t="str">
+      <c r="W184" s="23" t="str">
         <f t="shared" si="21"/>
         <v>B1</v>
       </c>
-      <c r="X184" s="34" t="str">
+      <c r="X184" s="23" t="str">
         <f t="shared" si="21"/>
         <v>B2</v>
       </c>
-      <c r="Y184" s="34" t="str">
+      <c r="Y184" s="24" t="str">
         <f t="shared" si="21"/>
         <v>B3</v>
       </c>
-      <c r="Z184" s="34" t="str">
+      <c r="Z184" s="25" t="str">
         <f t="shared" si="21"/>
         <v>B4</v>
       </c>
-      <c r="AA184" s="34" t="str">
+      <c r="AA184" s="23" t="str">
         <f t="shared" si="21"/>
         <v>B5</v>
       </c>
-      <c r="AB184" s="34" t="str">
+      <c r="AB184" s="35" t="str">
         <f t="shared" si="21"/>
         <v>B6</v>
       </c>
-      <c r="AC184" s="34" t="str">
+      <c r="AC184" s="35" t="str">
         <f t="shared" si="21"/>
         <v>B7</v>
       </c>
@@ -27956,95 +27965,95 @@
         <v>42</v>
       </c>
       <c r="F185" s="4"/>
-      <c r="G185" s="34" t="str">
+      <c r="G185" s="35" t="str">
         <f t="shared" ref="G185:AC185" si="22">DEC2HEX(G231)</f>
         <v>B8</v>
       </c>
-      <c r="H185" s="34" t="str">
+      <c r="H185" s="35" t="str">
         <f t="shared" si="22"/>
         <v>B9</v>
       </c>
-      <c r="I185" s="34" t="str">
+      <c r="I185" s="23" t="str">
         <f t="shared" si="22"/>
         <v>BA</v>
       </c>
-      <c r="J185" s="34" t="str">
+      <c r="J185" s="24" t="str">
         <f t="shared" si="22"/>
         <v>BB</v>
       </c>
-      <c r="K185" s="34" t="str">
+      <c r="K185" s="24" t="str">
         <f t="shared" si="22"/>
         <v>BC</v>
       </c>
-      <c r="L185" s="34" t="str">
+      <c r="L185" s="24" t="str">
         <f t="shared" si="22"/>
         <v>BD</v>
       </c>
-      <c r="M185" s="34" t="str">
+      <c r="M185" s="23" t="str">
         <f t="shared" si="22"/>
         <v>BE</v>
       </c>
-      <c r="N185" s="34" t="str">
+      <c r="N185" s="23" t="str">
         <f t="shared" si="22"/>
         <v>BF</v>
       </c>
-      <c r="O185" s="34" t="str">
+      <c r="O185" s="23" t="str">
         <f t="shared" si="22"/>
         <v>C0</v>
       </c>
-      <c r="P185" s="34" t="str">
+      <c r="P185" s="23" t="str">
         <f t="shared" si="22"/>
         <v>C1</v>
       </c>
-      <c r="Q185" s="34" t="str">
+      <c r="Q185" s="23" t="str">
         <f t="shared" si="22"/>
         <v>C2</v>
       </c>
-      <c r="R185" s="34" t="str">
+      <c r="R185" s="23" t="str">
         <f t="shared" si="22"/>
         <v>C3</v>
       </c>
-      <c r="S185" s="34" t="str">
+      <c r="S185" s="23" t="str">
         <f t="shared" si="22"/>
         <v>C4</v>
       </c>
-      <c r="T185" s="34" t="str">
+      <c r="T185" s="23" t="str">
         <f t="shared" si="22"/>
         <v>C5</v>
       </c>
-      <c r="U185" s="34" t="str">
+      <c r="U185" s="23" t="str">
         <f t="shared" si="22"/>
         <v>C6</v>
       </c>
-      <c r="V185" s="34" t="str">
+      <c r="V185" s="23" t="str">
         <f t="shared" si="22"/>
         <v>C7</v>
       </c>
-      <c r="W185" s="34" t="str">
+      <c r="W185" s="23" t="str">
         <f t="shared" si="22"/>
         <v>C8</v>
       </c>
-      <c r="X185" s="34" t="str">
+      <c r="X185" s="24" t="str">
         <f t="shared" si="22"/>
         <v>C9</v>
       </c>
-      <c r="Y185" s="34" t="str">
+      <c r="Y185" s="24" t="str">
         <f t="shared" si="22"/>
         <v>CA</v>
       </c>
-      <c r="Z185" s="34" t="str">
+      <c r="Z185" s="24" t="str">
         <f t="shared" si="22"/>
         <v>CB</v>
       </c>
-      <c r="AA185" s="34" t="str">
+      <c r="AA185" s="23" t="str">
         <f t="shared" si="22"/>
         <v>CC</v>
       </c>
-      <c r="AB185" s="34" t="str">
+      <c r="AB185" s="35" t="str">
         <f t="shared" si="22"/>
         <v>CD</v>
       </c>
-      <c r="AC185" s="34" t="str">
+      <c r="AC185" s="35" t="str">
         <f t="shared" si="22"/>
         <v>CE</v>
       </c>
@@ -28060,95 +28069,95 @@
         <v>183</v>
       </c>
       <c r="F186" s="4"/>
-      <c r="G186" s="34" t="str">
+      <c r="G186" s="35" t="str">
         <f t="shared" ref="G186:AC186" si="23">DEC2HEX(G232)</f>
         <v>CF</v>
       </c>
-      <c r="H186" s="34" t="str">
+      <c r="H186" s="35" t="str">
         <f t="shared" si="23"/>
         <v>D0</v>
       </c>
-      <c r="I186" s="34" t="str">
+      <c r="I186" s="28" t="str">
         <f t="shared" si="23"/>
         <v>D1</v>
       </c>
-      <c r="J186" s="34" t="str">
+      <c r="J186" s="24" t="str">
         <f t="shared" si="23"/>
         <v>D2</v>
       </c>
-      <c r="K186" s="34" t="str">
+      <c r="K186" s="24" t="str">
         <f t="shared" si="23"/>
         <v>D3</v>
       </c>
-      <c r="L186" s="34" t="str">
+      <c r="L186" s="24" t="str">
         <f t="shared" si="23"/>
         <v>D4</v>
       </c>
-      <c r="M186" s="34" t="str">
+      <c r="M186" s="23" t="str">
         <f t="shared" si="23"/>
         <v>D5</v>
       </c>
-      <c r="N186" s="34" t="str">
+      <c r="N186" s="23" t="str">
         <f t="shared" si="23"/>
         <v>D6</v>
       </c>
-      <c r="O186" s="34" t="str">
+      <c r="O186" s="23" t="str">
         <f t="shared" si="23"/>
         <v>D7</v>
       </c>
-      <c r="P186" s="34" t="str">
+      <c r="P186" s="23" t="str">
         <f t="shared" si="23"/>
         <v>D8</v>
       </c>
-      <c r="Q186" s="34" t="str">
+      <c r="Q186" s="23" t="str">
         <f t="shared" si="23"/>
         <v>D9</v>
       </c>
-      <c r="R186" s="34" t="str">
+      <c r="R186" s="30" t="str">
         <f t="shared" si="23"/>
         <v>DA</v>
       </c>
-      <c r="S186" s="34" t="str">
+      <c r="S186" s="23" t="str">
         <f t="shared" si="23"/>
         <v>DB</v>
       </c>
-      <c r="T186" s="34" t="str">
+      <c r="T186" s="23" t="str">
         <f t="shared" si="23"/>
         <v>DC</v>
       </c>
-      <c r="U186" s="34" t="str">
+      <c r="U186" s="23" t="str">
         <f t="shared" si="23"/>
         <v>DD</v>
       </c>
-      <c r="V186" s="34" t="str">
+      <c r="V186" s="23" t="str">
         <f t="shared" si="23"/>
         <v>DE</v>
       </c>
-      <c r="W186" s="34" t="str">
+      <c r="W186" s="23" t="str">
         <f t="shared" si="23"/>
         <v>DF</v>
       </c>
-      <c r="X186" s="34" t="str">
+      <c r="X186" s="24" t="str">
         <f t="shared" si="23"/>
         <v>E0</v>
       </c>
-      <c r="Y186" s="34" t="str">
+      <c r="Y186" s="24" t="str">
         <f t="shared" si="23"/>
         <v>E1</v>
       </c>
-      <c r="Z186" s="34" t="str">
+      <c r="Z186" s="24" t="str">
         <f t="shared" si="23"/>
         <v>E2</v>
       </c>
-      <c r="AA186" s="34" t="str">
+      <c r="AA186" s="28" t="str">
         <f t="shared" si="23"/>
         <v>E3</v>
       </c>
-      <c r="AB186" s="34" t="str">
+      <c r="AB186" s="35" t="str">
         <f t="shared" si="23"/>
         <v>E4</v>
       </c>
-      <c r="AC186" s="34" t="str">
+      <c r="AC186" s="35" t="str">
         <f t="shared" si="23"/>
         <v>E5</v>
       </c>
@@ -28164,95 +28173,95 @@
         <v>184</v>
       </c>
       <c r="F187" s="4"/>
-      <c r="G187" s="34" t="str">
+      <c r="G187" s="35" t="str">
         <f t="shared" ref="G187:AC187" si="24">DEC2HEX(G233)</f>
         <v>E6</v>
       </c>
-      <c r="H187" s="34" t="str">
+      <c r="H187" s="35" t="str">
         <f t="shared" si="24"/>
         <v>E7</v>
       </c>
-      <c r="I187" s="34" t="str">
+      <c r="I187" s="23" t="str">
         <f t="shared" si="24"/>
         <v>E8</v>
       </c>
-      <c r="J187" s="34" t="str">
+      <c r="J187" s="24" t="str">
         <f t="shared" si="24"/>
         <v>E9</v>
       </c>
-      <c r="K187" s="34" t="str">
+      <c r="K187" s="24" t="str">
         <f t="shared" si="24"/>
         <v>EA</v>
       </c>
-      <c r="L187" s="34" t="str">
+      <c r="L187" s="24" t="str">
         <f t="shared" si="24"/>
         <v>EB</v>
       </c>
-      <c r="M187" s="34" t="str">
+      <c r="M187" s="23" t="str">
         <f t="shared" si="24"/>
         <v>EC</v>
       </c>
-      <c r="N187" s="34" t="str">
+      <c r="N187" s="23" t="str">
         <f t="shared" si="24"/>
         <v>ED</v>
       </c>
-      <c r="O187" s="34" t="str">
+      <c r="O187" s="23" t="str">
         <f t="shared" si="24"/>
         <v>EE</v>
       </c>
-      <c r="P187" s="34" t="str">
+      <c r="P187" s="23" t="str">
         <f t="shared" si="24"/>
         <v>EF</v>
       </c>
-      <c r="Q187" s="34" t="str">
+      <c r="Q187" s="23" t="str">
         <f t="shared" si="24"/>
         <v>F0</v>
       </c>
-      <c r="R187" s="34" t="str">
+      <c r="R187" s="23" t="str">
         <f t="shared" si="24"/>
         <v>F1</v>
       </c>
-      <c r="S187" s="34" t="str">
+      <c r="S187" s="23" t="str">
         <f t="shared" si="24"/>
         <v>F2</v>
       </c>
-      <c r="T187" s="34" t="str">
+      <c r="T187" s="23" t="str">
         <f t="shared" si="24"/>
         <v>F3</v>
       </c>
-      <c r="U187" s="34" t="str">
+      <c r="U187" s="23" t="str">
         <f t="shared" si="24"/>
         <v>F4</v>
       </c>
-      <c r="V187" s="34" t="str">
+      <c r="V187" s="23" t="str">
         <f t="shared" si="24"/>
         <v>F5</v>
       </c>
-      <c r="W187" s="34" t="str">
+      <c r="W187" s="23" t="str">
         <f t="shared" si="24"/>
         <v>F6</v>
       </c>
-      <c r="X187" s="34" t="str">
+      <c r="X187" s="24" t="str">
         <f t="shared" si="24"/>
         <v>F7</v>
       </c>
-      <c r="Y187" s="34" t="str">
+      <c r="Y187" s="24" t="str">
         <f t="shared" si="24"/>
         <v>F8</v>
       </c>
-      <c r="Z187" s="34" t="str">
+      <c r="Z187" s="24" t="str">
         <f t="shared" si="24"/>
         <v>F9</v>
       </c>
-      <c r="AA187" s="34" t="str">
+      <c r="AA187" s="23" t="str">
         <f t="shared" si="24"/>
         <v>FA</v>
       </c>
-      <c r="AB187" s="34" t="str">
+      <c r="AB187" s="35" t="str">
         <f t="shared" si="24"/>
         <v>FB</v>
       </c>
-      <c r="AC187" s="34" t="str">
+      <c r="AC187" s="35" t="str">
         <f t="shared" si="24"/>
         <v>FC</v>
       </c>
@@ -28268,95 +28277,95 @@
         <v>185</v>
       </c>
       <c r="F188" s="4"/>
-      <c r="G188" s="34" t="str">
+      <c r="G188" s="35" t="str">
         <f t="shared" ref="G188:AC188" si="25">DEC2HEX(G234)</f>
         <v>FD</v>
       </c>
-      <c r="H188" s="34" t="str">
+      <c r="H188" s="35" t="str">
         <f t="shared" si="25"/>
         <v>FE</v>
       </c>
-      <c r="I188" s="34" t="str">
+      <c r="I188" s="23" t="str">
         <f t="shared" si="25"/>
         <v>FF</v>
       </c>
-      <c r="J188" s="34" t="str">
+      <c r="J188" s="25" t="str">
         <f t="shared" si="25"/>
         <v>100</v>
       </c>
-      <c r="K188" s="34" t="str">
+      <c r="K188" s="24" t="str">
         <f t="shared" si="25"/>
         <v>101</v>
       </c>
-      <c r="L188" s="34" t="str">
+      <c r="L188" s="29" t="str">
         <f t="shared" si="25"/>
         <v>102</v>
       </c>
-      <c r="M188" s="34" t="str">
+      <c r="M188" s="23" t="str">
         <f t="shared" si="25"/>
         <v>103</v>
       </c>
-      <c r="N188" s="34" t="str">
+      <c r="N188" s="23" t="str">
         <f t="shared" si="25"/>
         <v>104</v>
       </c>
-      <c r="O188" s="34" t="str">
+      <c r="O188" s="23" t="str">
         <f t="shared" si="25"/>
         <v>105</v>
       </c>
-      <c r="P188" s="34" t="str">
+      <c r="P188" s="23" t="str">
         <f t="shared" si="25"/>
         <v>106</v>
       </c>
-      <c r="Q188" s="34" t="str">
+      <c r="Q188" s="23" t="str">
         <f t="shared" si="25"/>
         <v>107</v>
       </c>
-      <c r="R188" s="34" t="str">
+      <c r="R188" s="23" t="str">
         <f t="shared" si="25"/>
         <v>108</v>
       </c>
-      <c r="S188" s="34" t="str">
+      <c r="S188" s="23" t="str">
         <f t="shared" si="25"/>
         <v>109</v>
       </c>
-      <c r="T188" s="34" t="str">
+      <c r="T188" s="23" t="str">
         <f t="shared" si="25"/>
         <v>10A</v>
       </c>
-      <c r="U188" s="34" t="str">
+      <c r="U188" s="23" t="str">
         <f t="shared" si="25"/>
         <v>10B</v>
       </c>
-      <c r="V188" s="34" t="str">
+      <c r="V188" s="23" t="str">
         <f t="shared" si="25"/>
         <v>10C</v>
       </c>
-      <c r="W188" s="34" t="str">
+      <c r="W188" s="23" t="str">
         <f t="shared" si="25"/>
         <v>10D</v>
       </c>
-      <c r="X188" s="34" t="str">
+      <c r="X188" s="23" t="str">
         <f t="shared" si="25"/>
         <v>10E</v>
       </c>
-      <c r="Y188" s="34" t="str">
+      <c r="Y188" s="24" t="str">
         <f t="shared" si="25"/>
         <v>10F</v>
       </c>
-      <c r="Z188" s="34" t="str">
+      <c r="Z188" s="25" t="str">
         <f t="shared" si="25"/>
         <v>110</v>
       </c>
-      <c r="AA188" s="34" t="str">
+      <c r="AA188" s="23" t="str">
         <f t="shared" si="25"/>
         <v>111</v>
       </c>
-      <c r="AB188" s="34" t="str">
+      <c r="AB188" s="35" t="str">
         <f t="shared" si="25"/>
         <v>112</v>
       </c>
-      <c r="AC188" s="34" t="str">
+      <c r="AC188" s="35" t="str">
         <f t="shared" si="25"/>
         <v>113</v>
       </c>
@@ -28372,95 +28381,95 @@
         <v>186</v>
       </c>
       <c r="F189" s="4"/>
-      <c r="G189" s="34" t="str">
+      <c r="G189" s="35" t="str">
         <f t="shared" ref="G189:AC189" si="26">DEC2HEX(G235)</f>
         <v>114</v>
       </c>
-      <c r="H189" s="34" t="str">
+      <c r="H189" s="35" t="str">
         <f t="shared" si="26"/>
         <v>115</v>
       </c>
-      <c r="I189" s="34" t="str">
+      <c r="I189" s="23" t="str">
         <f t="shared" si="26"/>
         <v>116</v>
       </c>
-      <c r="J189" s="34" t="str">
+      <c r="J189" s="24" t="str">
         <f t="shared" si="26"/>
         <v>117</v>
       </c>
-      <c r="K189" s="34" t="str">
+      <c r="K189" s="29" t="str">
         <f t="shared" si="26"/>
         <v>118</v>
       </c>
-      <c r="L189" s="34" t="str">
+      <c r="L189" s="29" t="str">
         <f t="shared" si="26"/>
         <v>119</v>
       </c>
-      <c r="M189" s="34" t="str">
+      <c r="M189" s="23" t="str">
         <f t="shared" si="26"/>
         <v>11A</v>
       </c>
-      <c r="N189" s="34" t="str">
+      <c r="N189" s="23" t="str">
         <f t="shared" si="26"/>
         <v>11B</v>
       </c>
-      <c r="O189" s="34" t="str">
+      <c r="O189" s="29" t="str">
         <f t="shared" si="26"/>
         <v>11C</v>
       </c>
-      <c r="P189" s="34" t="str">
+      <c r="P189" s="29" t="str">
         <f t="shared" si="26"/>
         <v>11D</v>
       </c>
-      <c r="Q189" s="34" t="str">
+      <c r="Q189" s="24" t="str">
         <f t="shared" si="26"/>
         <v>11E</v>
       </c>
-      <c r="R189" s="34" t="str">
+      <c r="R189" s="24" t="str">
         <f t="shared" si="26"/>
         <v>11F</v>
       </c>
-      <c r="S189" s="34" t="str">
+      <c r="S189" s="24" t="str">
         <f t="shared" si="26"/>
         <v>120</v>
       </c>
-      <c r="T189" s="34" t="str">
+      <c r="T189" s="29" t="str">
         <f t="shared" si="26"/>
         <v>121</v>
       </c>
-      <c r="U189" s="34" t="str">
+      <c r="U189" s="29" t="str">
         <f t="shared" si="26"/>
         <v>122</v>
       </c>
-      <c r="V189" s="34" t="str">
+      <c r="V189" s="23" t="str">
         <f t="shared" si="26"/>
         <v>123</v>
       </c>
-      <c r="W189" s="34" t="str">
+      <c r="W189" s="23" t="str">
         <f t="shared" si="26"/>
         <v>124</v>
       </c>
-      <c r="X189" s="34" t="str">
+      <c r="X189" s="23" t="str">
         <f t="shared" si="26"/>
         <v>125</v>
       </c>
-      <c r="Y189" s="34" t="str">
+      <c r="Y189" s="23" t="str">
         <f t="shared" si="26"/>
         <v>126</v>
       </c>
-      <c r="Z189" s="34" t="str">
+      <c r="Z189" s="24" t="str">
         <f t="shared" si="26"/>
         <v>127</v>
       </c>
-      <c r="AA189" s="34" t="str">
+      <c r="AA189" s="23" t="str">
         <f t="shared" si="26"/>
         <v>128</v>
       </c>
-      <c r="AB189" s="34" t="str">
+      <c r="AB189" s="35" t="str">
         <f t="shared" si="26"/>
         <v>129</v>
       </c>
-      <c r="AC189" s="34" t="str">
+      <c r="AC189" s="35" t="str">
         <f t="shared" si="26"/>
         <v>12A</v>
       </c>
@@ -28476,95 +28485,95 @@
         <v>187</v>
       </c>
       <c r="F190" s="4"/>
-      <c r="G190" s="34" t="str">
+      <c r="G190" s="35" t="str">
         <f t="shared" ref="G190:AC190" si="27">DEC2HEX(G236)</f>
         <v>12B</v>
       </c>
-      <c r="H190" s="34" t="str">
+      <c r="H190" s="35" t="str">
         <f t="shared" si="27"/>
         <v>12C</v>
       </c>
-      <c r="I190" s="34" t="str">
+      <c r="I190" s="23" t="str">
         <f t="shared" si="27"/>
         <v>12D</v>
       </c>
-      <c r="J190" s="34" t="str">
+      <c r="J190" s="23" t="str">
         <f t="shared" si="27"/>
         <v>12E</v>
       </c>
-      <c r="K190" s="34" t="str">
+      <c r="K190" s="23" t="str">
         <f t="shared" si="27"/>
         <v>12F</v>
       </c>
-      <c r="L190" s="34" t="str">
+      <c r="L190" s="23" t="str">
         <f t="shared" si="27"/>
         <v>130</v>
       </c>
-      <c r="M190" s="34" t="str">
+      <c r="M190" s="23" t="str">
         <f t="shared" si="27"/>
         <v>131</v>
       </c>
-      <c r="N190" s="34" t="str">
+      <c r="N190" s="23" t="str">
         <f t="shared" si="27"/>
         <v>132</v>
       </c>
-      <c r="O190" s="34" t="str">
+      <c r="O190" s="29" t="str">
         <f t="shared" si="27"/>
         <v>133</v>
       </c>
-      <c r="P190" s="34" t="str">
+      <c r="P190" s="24" t="str">
         <f t="shared" si="27"/>
         <v>134</v>
       </c>
-      <c r="Q190" s="34" t="str">
+      <c r="Q190" s="25" t="str">
         <f t="shared" si="27"/>
         <v>135</v>
       </c>
-      <c r="R190" s="34" t="str">
+      <c r="R190" s="24" t="str">
         <f t="shared" si="27"/>
         <v>136</v>
       </c>
-      <c r="S190" s="34" t="str">
+      <c r="S190" s="25" t="str">
         <f t="shared" si="27"/>
         <v>137</v>
       </c>
-      <c r="T190" s="34" t="str">
+      <c r="T190" s="24" t="str">
         <f t="shared" si="27"/>
         <v>138</v>
       </c>
-      <c r="U190" s="34" t="str">
+      <c r="U190" s="29" t="str">
         <f t="shared" si="27"/>
         <v>139</v>
       </c>
-      <c r="V190" s="34" t="str">
+      <c r="V190" s="23" t="str">
         <f t="shared" si="27"/>
         <v>13A</v>
       </c>
-      <c r="W190" s="34" t="str">
+      <c r="W190" s="23" t="str">
         <f t="shared" si="27"/>
         <v>13B</v>
       </c>
-      <c r="X190" s="34" t="str">
+      <c r="X190" s="23" t="str">
         <f t="shared" si="27"/>
         <v>13C</v>
       </c>
-      <c r="Y190" s="34" t="str">
+      <c r="Y190" s="23" t="str">
         <f t="shared" si="27"/>
         <v>13D</v>
       </c>
-      <c r="Z190" s="34" t="str">
+      <c r="Z190" s="23" t="str">
         <f t="shared" si="27"/>
         <v>13E</v>
       </c>
-      <c r="AA190" s="34" t="str">
+      <c r="AA190" s="23" t="str">
         <f t="shared" si="27"/>
         <v>13F</v>
       </c>
-      <c r="AB190" s="34" t="str">
+      <c r="AB190" s="35" t="str">
         <f t="shared" si="27"/>
         <v>140</v>
       </c>
-      <c r="AC190" s="34" t="str">
+      <c r="AC190" s="35" t="str">
         <f t="shared" si="27"/>
         <v>141</v>
       </c>
@@ -28580,95 +28589,95 @@
         <v>188</v>
       </c>
       <c r="F191" s="4"/>
-      <c r="G191" s="34" t="str">
+      <c r="G191" s="35" t="str">
         <f t="shared" ref="G191:AC191" si="28">DEC2HEX(G237)</f>
         <v>142</v>
       </c>
-      <c r="H191" s="34" t="str">
+      <c r="H191" s="35" t="str">
         <f t="shared" si="28"/>
         <v>143</v>
       </c>
-      <c r="I191" s="34" t="str">
+      <c r="I191" s="23" t="str">
         <f t="shared" si="28"/>
         <v>144</v>
       </c>
-      <c r="J191" s="34" t="str">
+      <c r="J191" s="23" t="str">
         <f t="shared" si="28"/>
         <v>145</v>
       </c>
-      <c r="K191" s="34" t="str">
+      <c r="K191" s="23" t="str">
         <f t="shared" si="28"/>
         <v>146</v>
       </c>
-      <c r="L191" s="34" t="str">
+      <c r="L191" s="23" t="str">
         <f t="shared" si="28"/>
         <v>147</v>
       </c>
-      <c r="M191" s="34" t="str">
+      <c r="M191" s="23" t="str">
         <f t="shared" si="28"/>
         <v>148</v>
       </c>
-      <c r="N191" s="34" t="str">
+      <c r="N191" s="23" t="str">
         <f t="shared" si="28"/>
         <v>149</v>
       </c>
-      <c r="O191" s="34" t="str">
+      <c r="O191" s="24" t="str">
         <f t="shared" si="28"/>
         <v>14A</v>
       </c>
-      <c r="P191" s="34" t="str">
+      <c r="P191" s="24" t="str">
         <f t="shared" si="28"/>
         <v>14B</v>
       </c>
-      <c r="Q191" s="34" t="str">
+      <c r="Q191" s="24" t="str">
         <f t="shared" si="28"/>
         <v>14C</v>
       </c>
-      <c r="R191" s="34" t="str">
+      <c r="R191" s="24" t="str">
         <f t="shared" si="28"/>
         <v>14D</v>
       </c>
-      <c r="S191" s="34" t="str">
+      <c r="S191" s="24" t="str">
         <f t="shared" si="28"/>
         <v>14E</v>
       </c>
-      <c r="T191" s="34" t="str">
+      <c r="T191" s="24" t="str">
         <f t="shared" si="28"/>
         <v>14F</v>
       </c>
-      <c r="U191" s="34" t="str">
+      <c r="U191" s="24" t="str">
         <f t="shared" si="28"/>
         <v>150</v>
       </c>
-      <c r="V191" s="34" t="str">
+      <c r="V191" s="23" t="str">
         <f t="shared" si="28"/>
         <v>151</v>
       </c>
-      <c r="W191" s="34" t="str">
+      <c r="W191" s="23" t="str">
         <f t="shared" si="28"/>
         <v>152</v>
       </c>
-      <c r="X191" s="34" t="str">
+      <c r="X191" s="23" t="str">
         <f t="shared" si="28"/>
         <v>153</v>
       </c>
-      <c r="Y191" s="34" t="str">
+      <c r="Y191" s="23" t="str">
         <f t="shared" si="28"/>
         <v>154</v>
       </c>
-      <c r="Z191" s="34" t="str">
+      <c r="Z191" s="23" t="str">
         <f t="shared" si="28"/>
         <v>155</v>
       </c>
-      <c r="AA191" s="34" t="str">
+      <c r="AA191" s="23" t="str">
         <f t="shared" si="28"/>
         <v>156</v>
       </c>
-      <c r="AB191" s="34" t="str">
+      <c r="AB191" s="35" t="str">
         <f t="shared" si="28"/>
         <v>157</v>
       </c>
-      <c r="AC191" s="34" t="str">
+      <c r="AC191" s="35" t="str">
         <f t="shared" si="28"/>
         <v>158</v>
       </c>
@@ -28680,95 +28689,95 @@
       </c>
       <c r="E192" s="4"/>
       <c r="F192" s="4"/>
-      <c r="G192" s="34" t="str">
+      <c r="G192" s="35" t="str">
         <f t="shared" ref="G192:AC192" si="29">DEC2HEX(G238)</f>
         <v>159</v>
       </c>
-      <c r="H192" s="34" t="str">
+      <c r="H192" s="35" t="str">
         <f t="shared" si="29"/>
         <v>15A</v>
       </c>
-      <c r="I192" s="34" t="str">
+      <c r="I192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>15B</v>
       </c>
-      <c r="J192" s="34" t="str">
+      <c r="J192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>15C</v>
       </c>
-      <c r="K192" s="34" t="str">
+      <c r="K192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>15D</v>
       </c>
-      <c r="L192" s="34" t="str">
+      <c r="L192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>15E</v>
       </c>
-      <c r="M192" s="34" t="str">
+      <c r="M192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>15F</v>
       </c>
-      <c r="N192" s="34" t="str">
+      <c r="N192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>160</v>
       </c>
-      <c r="O192" s="34" t="str">
+      <c r="O192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>161</v>
       </c>
-      <c r="P192" s="34" t="str">
+      <c r="P192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>162</v>
       </c>
-      <c r="Q192" s="34" t="str">
+      <c r="Q192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>163</v>
       </c>
-      <c r="R192" s="34" t="str">
+      <c r="R192" s="28" t="str">
         <f t="shared" si="29"/>
         <v>164</v>
       </c>
-      <c r="S192" s="34" t="str">
+      <c r="S192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>165</v>
       </c>
-      <c r="T192" s="34" t="str">
+      <c r="T192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>166</v>
       </c>
-      <c r="U192" s="34" t="str">
+      <c r="U192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>167</v>
       </c>
-      <c r="V192" s="34" t="str">
+      <c r="V192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>168</v>
       </c>
-      <c r="W192" s="34" t="str">
+      <c r="W192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>169</v>
       </c>
-      <c r="X192" s="34" t="str">
+      <c r="X192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>16A</v>
       </c>
-      <c r="Y192" s="34" t="str">
+      <c r="Y192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>16B</v>
       </c>
-      <c r="Z192" s="34" t="str">
+      <c r="Z192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>16C</v>
       </c>
-      <c r="AA192" s="34" t="str">
+      <c r="AA192" s="23" t="str">
         <f t="shared" si="29"/>
         <v>16D</v>
       </c>
-      <c r="AB192" s="34" t="str">
+      <c r="AB192" s="35" t="str">
         <f t="shared" si="29"/>
         <v>16E</v>
       </c>
-      <c r="AC192" s="34" t="str">
+      <c r="AC192" s="35" t="str">
         <f t="shared" si="29"/>
         <v>16F</v>
       </c>
@@ -28780,95 +28789,95 @@
       </c>
       <c r="E193" s="4"/>
       <c r="F193" s="4"/>
-      <c r="G193" s="34" t="str">
+      <c r="G193" s="35" t="str">
         <f t="shared" ref="G193:AC193" si="30">DEC2HEX(G239)</f>
         <v>170</v>
       </c>
-      <c r="H193" s="34" t="str">
+      <c r="H193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>171</v>
       </c>
-      <c r="I193" s="34" t="str">
+      <c r="I193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>172</v>
       </c>
-      <c r="J193" s="34" t="str">
+      <c r="J193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>173</v>
       </c>
-      <c r="K193" s="34" t="str">
+      <c r="K193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>174</v>
       </c>
-      <c r="L193" s="34" t="str">
+      <c r="L193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>175</v>
       </c>
-      <c r="M193" s="34" t="str">
+      <c r="M193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>176</v>
       </c>
-      <c r="N193" s="34" t="str">
+      <c r="N193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>177</v>
       </c>
-      <c r="O193" s="34" t="str">
+      <c r="O193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>178</v>
       </c>
-      <c r="P193" s="34" t="str">
+      <c r="P193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>179</v>
       </c>
-      <c r="Q193" s="34" t="str">
+      <c r="Q193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>17A</v>
       </c>
-      <c r="R193" s="34" t="str">
+      <c r="R193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>17B</v>
       </c>
-      <c r="S193" s="34" t="str">
+      <c r="S193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>17C</v>
       </c>
-      <c r="T193" s="34" t="str">
+      <c r="T193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>17D</v>
       </c>
-      <c r="U193" s="34" t="str">
+      <c r="U193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>17E</v>
       </c>
-      <c r="V193" s="34" t="str">
+      <c r="V193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>17F</v>
       </c>
-      <c r="W193" s="34" t="str">
+      <c r="W193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>180</v>
       </c>
-      <c r="X193" s="34" t="str">
+      <c r="X193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>181</v>
       </c>
-      <c r="Y193" s="34" t="str">
+      <c r="Y193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>182</v>
       </c>
-      <c r="Z193" s="34" t="str">
+      <c r="Z193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>183</v>
       </c>
-      <c r="AA193" s="34" t="str">
+      <c r="AA193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>184</v>
       </c>
-      <c r="AB193" s="34" t="str">
+      <c r="AB193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>185</v>
       </c>
-      <c r="AC193" s="34" t="str">
+      <c r="AC193" s="35" t="str">
         <f t="shared" si="30"/>
         <v>186</v>
       </c>
@@ -28880,95 +28889,95 @@
       </c>
       <c r="E194" s="4"/>
       <c r="F194" s="4"/>
-      <c r="G194" s="34" t="str">
+      <c r="G194" s="35" t="str">
         <f t="shared" ref="G194:AC194" si="31">DEC2HEX(G240)</f>
         <v>187</v>
       </c>
-      <c r="H194" s="34" t="str">
+      <c r="H194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>188</v>
       </c>
-      <c r="I194" s="34" t="str">
+      <c r="I194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>189</v>
       </c>
-      <c r="J194" s="34" t="str">
+      <c r="J194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>18A</v>
       </c>
-      <c r="K194" s="34" t="str">
+      <c r="K194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>18B</v>
       </c>
-      <c r="L194" s="34" t="str">
+      <c r="L194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>18C</v>
       </c>
-      <c r="M194" s="34" t="str">
+      <c r="M194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>18D</v>
       </c>
-      <c r="N194" s="34" t="str">
+      <c r="N194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>18E</v>
       </c>
-      <c r="O194" s="34" t="str">
+      <c r="O194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>18F</v>
       </c>
-      <c r="P194" s="34" t="str">
+      <c r="P194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>190</v>
       </c>
-      <c r="Q194" s="34" t="str">
+      <c r="Q194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>191</v>
       </c>
-      <c r="R194" s="34" t="str">
+      <c r="R194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>192</v>
       </c>
-      <c r="S194" s="34" t="str">
+      <c r="S194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>193</v>
       </c>
-      <c r="T194" s="34" t="str">
+      <c r="T194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>194</v>
       </c>
-      <c r="U194" s="34" t="str">
+      <c r="U194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>195</v>
       </c>
-      <c r="V194" s="34" t="str">
+      <c r="V194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>196</v>
       </c>
-      <c r="W194" s="34" t="str">
+      <c r="W194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>197</v>
       </c>
-      <c r="X194" s="34" t="str">
+      <c r="X194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>198</v>
       </c>
-      <c r="Y194" s="34" t="str">
+      <c r="Y194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>199</v>
       </c>
-      <c r="Z194" s="34" t="str">
+      <c r="Z194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>19A</v>
       </c>
-      <c r="AA194" s="34" t="str">
+      <c r="AA194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>19B</v>
       </c>
-      <c r="AB194" s="34" t="str">
+      <c r="AB194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>19C</v>
       </c>
-      <c r="AC194" s="34" t="str">
+      <c r="AC194" s="35" t="str">
         <f t="shared" si="31"/>
         <v>19D</v>
       </c>

</xml_diff>

<commit_message>
##STABLE## ELS spreadsheet updated.
</commit_message>
<xml_diff>
--- a/Map_Shapes/Map/() darkness/TOD, ELS, PLS Charts v0.01.xlsx
+++ b/Map_Shapes/Map/() darkness/TOD, ELS, PLS Charts v0.01.xlsx
@@ -19927,7 +19927,7 @@
   <dimension ref="A1:BS288"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C225" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G262" sqref="G262"/>
+      <selection activeCell="J248" sqref="J248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31151,7 +31151,7 @@
         <f>DEC2HEX(AD270)</f>
         <v>17</v>
       </c>
-      <c r="AE244" s="40" t="str">
+      <c r="AE244" s="35" t="str">
         <f>DEC2HEX(AE270)</f>
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
DEV: code mostly written for CALCULATE.ELS.LIGHT_ONSCREEN optimization.
</commit_message>
<xml_diff>
--- a/Map_Shapes/Map/() darkness/TOD, ELS, PLS Charts v0.01.xlsx
+++ b/Map_Shapes/Map/() darkness/TOD, ELS, PLS Charts v0.01.xlsx
@@ -1280,7 +1280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K88" authorId="0">
+    <comment ref="M88" authorId="0">
       <text>
         <r>
           <rPr>
@@ -20463,10 +20463,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BS444"/>
+  <dimension ref="A1:BS493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="V117" sqref="V117"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K88" sqref="K88:L88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24484,55 +24484,55 @@
         <v>0</v>
       </c>
       <c r="F88" s="33"/>
-      <c r="K88" s="38" t="s">
+      <c r="M88" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="L88" s="38" t="s">
+      <c r="N88" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="M88" s="38" t="s">
+      <c r="O88" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="N88" s="38" t="s">
+      <c r="P88" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="O88" s="38" t="s">
+      <c r="Q88" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="P88" s="38" t="s">
+      <c r="R88" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="Q88" s="38" t="s">
+      <c r="S88" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="R88" s="38" t="s">
+      <c r="T88" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="S88" s="44" t="s">
+      <c r="U88" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="T88" s="38" t="s">
+      <c r="V88" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="U88" s="38" t="s">
+      <c r="W88" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="V88" s="38" t="s">
+      <c r="X88" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="W88" s="38" t="s">
+      <c r="Y88" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="X88" s="1" t="s">
+      <c r="Z88" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="Y88" s="1" t="s">
+      <c r="AA88" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="Z88" s="1" t="s">
+      <c r="AB88" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AA88" s="1" t="s">
+      <c r="AC88" s="1" t="s">
         <v>111</v>
       </c>
     </row>
@@ -25698,7 +25698,7 @@
       <c r="BO95" s="35"/>
       <c r="BP95" s="63"/>
     </row>
-    <row r="96" spans="1:68">
+    <row r="96" spans="1:68" ht="14.25" customHeight="1">
       <c r="A96" s="17" t="s">
         <v>85</v>
       </c>
@@ -34483,7 +34483,10 @@
         <v>233</v>
       </c>
     </row>
-    <row r="227" spans="1:26" ht="23.25">
+    <row r="224" spans="1:5" hidden="1"/>
+    <row r="225" spans="1:26" hidden="1"/>
+    <row r="226" spans="1:26" hidden="1"/>
+    <row r="227" spans="1:26" ht="23.25" hidden="1">
       <c r="A227" s="13" t="s">
         <v>223</v>
       </c>
@@ -34493,7 +34496,7 @@
       <c r="F227" s="27"/>
       <c r="G227" s="27"/>
     </row>
-    <row r="228" spans="1:26" ht="18.75">
+    <row r="228" spans="1:26" ht="18.75" hidden="1">
       <c r="A228" t="s">
         <v>206</v>
       </c>
@@ -34501,10 +34504,10 @@
         <v>204</v>
       </c>
     </row>
-    <row r="229" spans="1:26" ht="18.75">
+    <row r="229" spans="1:26" ht="18.75" hidden="1">
       <c r="L229" s="18"/>
     </row>
-    <row r="230" spans="1:26" ht="18.75">
+    <row r="230" spans="1:26" ht="18.75" hidden="1">
       <c r="A230" t="s">
         <v>221</v>
       </c>
@@ -34517,19 +34520,19 @@
       </c>
       <c r="L230" s="18"/>
     </row>
-    <row r="231" spans="1:26" ht="18.75">
+    <row r="231" spans="1:26" ht="18.75" hidden="1">
       <c r="L231" s="18"/>
     </row>
-    <row r="232" spans="1:26" ht="18.75">
+    <row r="232" spans="1:26" ht="18.75" hidden="1">
       <c r="L232" s="18"/>
     </row>
-    <row r="233" spans="1:26" ht="18.75">
+    <row r="233" spans="1:26" ht="18.75" hidden="1">
       <c r="L233" s="18"/>
     </row>
-    <row r="234" spans="1:26" ht="18.75">
+    <row r="234" spans="1:26" ht="18.75" hidden="1">
       <c r="L234" s="18"/>
     </row>
-    <row r="235" spans="1:26">
+    <row r="235" spans="1:26" hidden="1">
       <c r="I235" s="6" t="s">
         <v>82</v>
       </c>
@@ -34585,7 +34588,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="236" spans="1:26">
+    <row r="236" spans="1:26" hidden="1">
       <c r="A236" s="5" t="s">
         <v>94</v>
       </c>
@@ -34644,7 +34647,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="237" spans="1:26">
+    <row r="237" spans="1:26" hidden="1">
       <c r="D237" s="6" t="s">
         <v>112</v>
       </c>
@@ -34656,7 +34659,7 @@
       <c r="H237" s="33"/>
       <c r="R237" s="28"/>
     </row>
-    <row r="238" spans="1:26">
+    <row r="238" spans="1:26" hidden="1">
       <c r="A238" t="s">
         <v>93</v>
       </c>
@@ -34722,7 +34725,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="239" spans="1:26">
+    <row r="239" spans="1:26" hidden="1">
       <c r="A239" s="17" t="s">
         <v>83</v>
       </c>
@@ -34788,7 +34791,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="240" spans="1:26">
+    <row r="240" spans="1:26" hidden="1">
       <c r="A240" s="17" t="s">
         <v>84</v>
       </c>
@@ -34854,7 +34857,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="241" spans="1:26">
+    <row r="241" spans="1:26" hidden="1">
       <c r="A241" s="17" t="s">
         <v>85</v>
       </c>
@@ -34920,7 +34923,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="242" spans="1:26">
+    <row r="242" spans="1:26" hidden="1">
       <c r="A242" s="17" t="s">
         <v>86</v>
       </c>
@@ -34986,7 +34989,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="243" spans="1:26">
+    <row r="243" spans="1:26" hidden="1">
       <c r="A243" s="17" t="s">
         <v>87</v>
       </c>
@@ -35052,7 +35055,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="244" spans="1:26">
+    <row r="244" spans="1:26" hidden="1">
       <c r="A244" s="14" t="s">
         <v>88</v>
       </c>
@@ -35118,7 +35121,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="245" spans="1:26">
+    <row r="245" spans="1:26" hidden="1">
       <c r="A245" s="14" t="s">
         <v>89</v>
       </c>
@@ -35184,7 +35187,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="246" spans="1:26">
+    <row r="246" spans="1:26" hidden="1">
       <c r="A246" s="14" t="s">
         <v>90</v>
       </c>
@@ -35250,7 +35253,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="247" spans="1:26">
+    <row r="247" spans="1:26" hidden="1">
       <c r="A247" s="14" t="s">
         <v>91</v>
       </c>
@@ -35316,7 +35319,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="248" spans="1:26">
+    <row r="248" spans="1:26" hidden="1">
       <c r="A248" s="14" t="s">
         <v>92</v>
       </c>
@@ -35382,7 +35385,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="249" spans="1:26">
+    <row r="249" spans="1:26" hidden="1">
       <c r="D249" s="8"/>
       <c r="E249" s="4"/>
       <c r="F249" s="4"/>
@@ -35391,7 +35394,7 @@
       <c r="I249" s="3"/>
       <c r="R249" s="28"/>
     </row>
-    <row r="250" spans="1:26">
+    <row r="250" spans="1:26" hidden="1">
       <c r="D250" s="7"/>
       <c r="E250" s="2"/>
       <c r="F250" s="2"/>
@@ -35416,15 +35419,15 @@
       <c r="Y250" s="2"/>
       <c r="Z250" s="2"/>
     </row>
-    <row r="251" spans="1:26">
+    <row r="251" spans="1:26" hidden="1">
       <c r="I251" s="5"/>
     </row>
-    <row r="252" spans="1:26" ht="18.75">
+    <row r="252" spans="1:26" ht="18.75" hidden="1">
       <c r="L252" s="18" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="253" spans="1:26">
+    <row r="253" spans="1:26" hidden="1">
       <c r="I253" s="6" t="s">
         <v>82</v>
       </c>
@@ -35480,7 +35483,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="254" spans="1:26">
+    <row r="254" spans="1:26" hidden="1">
       <c r="A254" s="5" t="s">
         <v>94</v>
       </c>
@@ -35539,7 +35542,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="255" spans="1:26">
+    <row r="255" spans="1:26" hidden="1">
       <c r="D255" s="6" t="s">
         <v>112</v>
       </c>
@@ -35550,7 +35553,7 @@
       <c r="G255" s="33"/>
       <c r="H255" s="33"/>
     </row>
-    <row r="256" spans="1:26">
+    <row r="256" spans="1:26" hidden="1">
       <c r="A256" t="s">
         <v>93</v>
       </c>
@@ -35616,7 +35619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:27">
+    <row r="257" spans="1:27" hidden="1">
       <c r="A257" s="17" t="s">
         <v>83</v>
       </c>
@@ -35682,7 +35685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:27">
+    <row r="258" spans="1:27" hidden="1">
       <c r="A258" s="17" t="s">
         <v>84</v>
       </c>
@@ -35748,7 +35751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:27">
+    <row r="259" spans="1:27" hidden="1">
       <c r="A259" s="17" t="s">
         <v>85</v>
       </c>
@@ -35814,7 +35817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:27">
+    <row r="260" spans="1:27" hidden="1">
       <c r="A260" s="17" t="s">
         <v>86</v>
       </c>
@@ -35880,7 +35883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:27">
+    <row r="261" spans="1:27" hidden="1">
       <c r="A261" s="17" t="s">
         <v>87</v>
       </c>
@@ -35947,7 +35950,7 @@
       </c>
       <c r="AA261" s="28"/>
     </row>
-    <row r="262" spans="1:27">
+    <row r="262" spans="1:27" hidden="1">
       <c r="A262" s="14" t="s">
         <v>88</v>
       </c>
@@ -36013,7 +36016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:27">
+    <row r="263" spans="1:27" hidden="1">
       <c r="A263" s="14" t="s">
         <v>89</v>
       </c>
@@ -36079,7 +36082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:27">
+    <row r="264" spans="1:27" hidden="1">
       <c r="A264" s="14" t="s">
         <v>90</v>
       </c>
@@ -36145,7 +36148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:27">
+    <row r="265" spans="1:27" hidden="1">
       <c r="A265" s="14" t="s">
         <v>91</v>
       </c>
@@ -36211,7 +36214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:27">
+    <row r="266" spans="1:27" hidden="1">
       <c r="A266" s="14" t="s">
         <v>92</v>
       </c>
@@ -36277,7 +36280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:27">
+    <row r="267" spans="1:27" hidden="1">
       <c r="D267" s="8"/>
       <c r="E267" s="4"/>
       <c r="F267" s="4"/>
@@ -36285,12 +36288,13 @@
       <c r="H267" s="4"/>
       <c r="I267" s="3"/>
     </row>
-    <row r="269" spans="1:27">
+    <row r="268" spans="1:27" hidden="1"/>
+    <row r="269" spans="1:27" hidden="1">
       <c r="A269" s="5" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="270" spans="1:27">
+    <row r="270" spans="1:27" hidden="1">
       <c r="E270" t="s">
         <v>209</v>
       </c>
@@ -36363,7 +36367,7 @@
         <v>01</v>
       </c>
     </row>
-    <row r="271" spans="1:27">
+    <row r="271" spans="1:27" hidden="1">
       <c r="J271" t="str">
         <f>CONCATENATE("0",J257)</f>
         <v>01</v>
@@ -36433,7 +36437,7 @@
         <v>01</v>
       </c>
     </row>
-    <row r="272" spans="1:27">
+    <row r="272" spans="1:27" hidden="1">
       <c r="J272" t="str">
         <f t="shared" ref="J272:Z278" si="70">CONCATENATE("0",J258)</f>
         <v>00</v>
@@ -36503,7 +36507,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="273" spans="5:26">
+    <row r="273" spans="5:26" hidden="1">
       <c r="J273" t="str">
         <f t="shared" si="70"/>
         <v>00</v>
@@ -36573,7 +36577,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="274" spans="5:26">
+    <row r="274" spans="5:26" hidden="1">
       <c r="J274" t="str">
         <f t="shared" si="70"/>
         <v>00</v>
@@ -36643,7 +36647,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="275" spans="5:26">
+    <row r="275" spans="5:26" hidden="1">
       <c r="J275" t="str">
         <f t="shared" si="70"/>
         <v>00</v>
@@ -36713,7 +36717,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="276" spans="5:26">
+    <row r="276" spans="5:26" hidden="1">
       <c r="J276" t="str">
         <f t="shared" si="70"/>
         <v>00</v>
@@ -36783,7 +36787,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="277" spans="5:26">
+    <row r="277" spans="5:26" hidden="1">
       <c r="J277" t="str">
         <f>CONCATENATE("0",J263)</f>
         <v>00</v>
@@ -36853,7 +36857,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="278" spans="5:26">
+    <row r="278" spans="5:26" hidden="1">
       <c r="J278" t="str">
         <f>CONCATENATE("0",J264)</f>
         <v>00</v>
@@ -36923,7 +36927,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="279" spans="5:26">
+    <row r="279" spans="5:26" hidden="1">
       <c r="J279" t="str">
         <f t="shared" ref="J279:Z280" si="71">CONCATENATE("0",J265)</f>
         <v>01</v>
@@ -36993,7 +36997,7 @@
         <v>01</v>
       </c>
     </row>
-    <row r="280" spans="5:26">
+    <row r="280" spans="5:26" hidden="1">
       <c r="J280" t="str">
         <f t="shared" si="71"/>
         <v>01</v>
@@ -37063,7 +37067,8 @@
         <v>01</v>
       </c>
     </row>
-    <row r="282" spans="5:26">
+    <row r="281" spans="5:26" hidden="1"/>
+    <row r="282" spans="5:26" hidden="1">
       <c r="E282" s="9" t="s">
         <v>210</v>
       </c>
@@ -37071,7 +37076,7 @@
       <c r="G282" s="9"/>
       <c r="H282" s="9"/>
     </row>
-    <row r="283" spans="5:26">
+    <row r="283" spans="5:26" hidden="1">
       <c r="J283" t="str">
         <f>J270</f>
         <v>01</v>
@@ -37141,7 +37146,7 @@
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01</v>
       </c>
     </row>
-    <row r="284" spans="5:26">
+    <row r="284" spans="5:26" hidden="1">
       <c r="J284" t="str">
         <f>CONCATENATE(Z283,".",J271)</f>
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01</v>
@@ -37211,7 +37216,7 @@
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01</v>
       </c>
     </row>
-    <row r="285" spans="5:26">
+    <row r="285" spans="5:26" hidden="1">
       <c r="J285" t="str">
         <f t="shared" ref="J285:J293" si="73">CONCATENATE(Z284,".",J272)</f>
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00</v>
@@ -37281,7 +37286,7 @@
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00</v>
       </c>
     </row>
-    <row r="286" spans="5:26">
+    <row r="286" spans="5:26" hidden="1">
       <c r="J286" t="str">
         <f t="shared" si="73"/>
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00</v>
@@ -37351,7 +37356,7 @@
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00</v>
       </c>
     </row>
-    <row r="287" spans="5:26">
+    <row r="287" spans="5:26" hidden="1">
       <c r="J287" t="str">
         <f t="shared" si="73"/>
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00</v>
@@ -37421,7 +37426,7 @@
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00</v>
       </c>
     </row>
-    <row r="288" spans="5:26">
+    <row r="288" spans="5:26" hidden="1">
       <c r="J288" t="str">
         <f t="shared" si="73"/>
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00</v>
@@ -37491,7 +37496,7 @@
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00</v>
       </c>
     </row>
-    <row r="289" spans="10:26">
+    <row r="289" spans="10:26" hidden="1">
       <c r="J289" t="str">
         <f t="shared" si="73"/>
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00</v>
@@ -37561,7 +37566,7 @@
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00</v>
       </c>
     </row>
-    <row r="290" spans="10:26">
+    <row r="290" spans="10:26" hidden="1">
       <c r="J290" t="str">
         <f t="shared" si="73"/>
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00</v>
@@ -37631,7 +37636,7 @@
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00</v>
       </c>
     </row>
-    <row r="291" spans="10:26">
+    <row r="291" spans="10:26" hidden="1">
       <c r="J291" t="str">
         <f t="shared" si="73"/>
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00</v>
@@ -37701,7 +37706,7 @@
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00</v>
       </c>
     </row>
-    <row r="292" spans="10:26">
+    <row r="292" spans="10:26" hidden="1">
       <c r="J292" t="str">
         <f t="shared" si="73"/>
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01</v>
@@ -37771,7 +37776,7 @@
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01</v>
       </c>
     </row>
-    <row r="293" spans="10:26">
+    <row r="293" spans="10:26" hidden="1">
       <c r="J293" t="str">
         <f t="shared" si="73"/>
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01</v>
@@ -37841,7 +37846,21 @@
         <v>01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.00.00.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.00.00.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.00.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01.01</v>
       </c>
     </row>
-    <row r="308" spans="1:4" ht="23.25">
+    <row r="294" spans="10:26" hidden="1"/>
+    <row r="295" spans="10:26" hidden="1"/>
+    <row r="296" spans="10:26" hidden="1"/>
+    <row r="297" spans="10:26" hidden="1"/>
+    <row r="298" spans="10:26" hidden="1"/>
+    <row r="299" spans="10:26" hidden="1"/>
+    <row r="300" spans="10:26" hidden="1"/>
+    <row r="301" spans="10:26" hidden="1"/>
+    <row r="302" spans="10:26" hidden="1"/>
+    <row r="303" spans="10:26" hidden="1"/>
+    <row r="304" spans="10:26" hidden="1"/>
+    <row r="305" spans="1:4" hidden="1"/>
+    <row r="306" spans="1:4" hidden="1"/>
+    <row r="307" spans="1:4" hidden="1"/>
+    <row r="308" spans="1:4" ht="23.25" hidden="1">
       <c r="A308" s="31" t="s">
         <v>224</v>
       </c>
@@ -37849,17 +37868,30 @@
       <c r="C308" s="27"/>
       <c r="D308" s="27"/>
     </row>
-    <row r="321" spans="1:29" ht="23.25">
+    <row r="309" spans="1:4" hidden="1"/>
+    <row r="310" spans="1:4" hidden="1"/>
+    <row r="311" spans="1:4" hidden="1"/>
+    <row r="312" spans="1:4" hidden="1"/>
+    <row r="313" spans="1:4" hidden="1"/>
+    <row r="314" spans="1:4" hidden="1"/>
+    <row r="315" spans="1:4" hidden="1"/>
+    <row r="316" spans="1:4" hidden="1"/>
+    <row r="317" spans="1:4" hidden="1"/>
+    <row r="318" spans="1:4" hidden="1"/>
+    <row r="319" spans="1:4" hidden="1"/>
+    <row r="320" spans="1:4" hidden="1"/>
+    <row r="321" spans="1:29" ht="23.25" hidden="1">
       <c r="A321" s="13" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="323" spans="1:29" ht="23.25">
+    <row r="322" spans="1:29" hidden="1"/>
+    <row r="323" spans="1:29" ht="23.25" hidden="1">
       <c r="A323" s="13" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="324" spans="1:29" ht="18.75">
+    <row r="324" spans="1:29" ht="18.75" hidden="1">
       <c r="A324" t="s">
         <v>206</v>
       </c>
@@ -37867,10 +37899,10 @@
         <v>204</v>
       </c>
     </row>
-    <row r="325" spans="1:29" ht="18.75">
+    <row r="325" spans="1:29" ht="18.75" hidden="1">
       <c r="L325" s="18"/>
     </row>
-    <row r="326" spans="1:29" ht="18.75">
+    <row r="326" spans="1:29" ht="18.75" hidden="1">
       <c r="A326" t="s">
         <v>221</v>
       </c>
@@ -37883,19 +37915,19 @@
       </c>
       <c r="L326" s="18"/>
     </row>
-    <row r="327" spans="1:29" ht="18.75">
+    <row r="327" spans="1:29" ht="18.75" hidden="1">
       <c r="L327" s="18"/>
     </row>
-    <row r="328" spans="1:29" ht="18.75">
+    <row r="328" spans="1:29" ht="18.75" hidden="1">
       <c r="L328" s="18"/>
     </row>
-    <row r="329" spans="1:29" ht="18.75">
+    <row r="329" spans="1:29" ht="18.75" hidden="1">
       <c r="L329" s="18"/>
     </row>
-    <row r="330" spans="1:29" ht="18.75">
+    <row r="330" spans="1:29" ht="18.75" hidden="1">
       <c r="L330" s="18"/>
     </row>
-    <row r="331" spans="1:29">
+    <row r="331" spans="1:29" hidden="1">
       <c r="F331" s="6" t="s">
         <v>82</v>
       </c>
@@ -37951,7 +37983,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="332" spans="1:29">
+    <row r="332" spans="1:29" hidden="1">
       <c r="A332" s="5" t="s">
         <v>94</v>
       </c>
@@ -38028,7 +38060,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="333" spans="1:29">
+    <row r="333" spans="1:29" hidden="1">
       <c r="D333" s="6" t="s">
         <v>112</v>
       </c>
@@ -38129,7 +38161,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="334" spans="1:29">
+    <row r="334" spans="1:29" hidden="1">
       <c r="D334" s="32">
         <v>-3</v>
       </c>
@@ -38228,7 +38260,7 @@
         <v>2D</v>
       </c>
     </row>
-    <row r="335" spans="1:29">
+    <row r="335" spans="1:29" hidden="1">
       <c r="D335" s="32">
         <v>-2</v>
       </c>
@@ -38327,7 +38359,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="336" spans="1:29">
+    <row r="336" spans="1:29" hidden="1">
       <c r="D336" s="32">
         <v>-1</v>
       </c>
@@ -38426,7 +38458,7 @@
         <v>5B</v>
       </c>
     </row>
-    <row r="337" spans="1:29">
+    <row r="337" spans="1:29" hidden="1">
       <c r="A337" t="s">
         <v>93</v>
       </c>
@@ -38530,7 +38562,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="338" spans="1:29">
+    <row r="338" spans="1:29" hidden="1">
       <c r="A338" s="17" t="s">
         <v>83</v>
       </c>
@@ -38634,7 +38666,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="339" spans="1:29">
+    <row r="339" spans="1:29" hidden="1">
       <c r="A339" s="17" t="s">
         <v>84</v>
       </c>
@@ -38738,7 +38770,7 @@
         <v>A0</v>
       </c>
     </row>
-    <row r="340" spans="1:29">
+    <row r="340" spans="1:29" hidden="1">
       <c r="A340" s="17" t="s">
         <v>85</v>
       </c>
@@ -38842,7 +38874,7 @@
         <v>B7</v>
       </c>
     </row>
-    <row r="341" spans="1:29">
+    <row r="341" spans="1:29" hidden="1">
       <c r="A341" s="17" t="s">
         <v>86</v>
       </c>
@@ -38946,7 +38978,7 @@
         <v>CE</v>
       </c>
     </row>
-    <row r="342" spans="1:29">
+    <row r="342" spans="1:29" hidden="1">
       <c r="A342" s="17" t="s">
         <v>87</v>
       </c>
@@ -39050,7 +39082,7 @@
         <v>E5</v>
       </c>
     </row>
-    <row r="343" spans="1:29">
+    <row r="343" spans="1:29" hidden="1">
       <c r="A343" s="14" t="s">
         <v>88</v>
       </c>
@@ -39154,7 +39186,7 @@
         <v>FC</v>
       </c>
     </row>
-    <row r="344" spans="1:29">
+    <row r="344" spans="1:29" hidden="1">
       <c r="A344" s="14" t="s">
         <v>89</v>
       </c>
@@ -39258,7 +39290,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="345" spans="1:29">
+    <row r="345" spans="1:29" hidden="1">
       <c r="A345" s="14" t="s">
         <v>90</v>
       </c>
@@ -39362,7 +39394,7 @@
         <v>12A</v>
       </c>
     </row>
-    <row r="346" spans="1:29">
+    <row r="346" spans="1:29" hidden="1">
       <c r="A346" s="14" t="s">
         <v>91</v>
       </c>
@@ -39466,7 +39498,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="347" spans="1:29">
+    <row r="347" spans="1:29" hidden="1">
       <c r="A347" s="14" t="s">
         <v>92</v>
       </c>
@@ -39570,7 +39602,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="348" spans="1:29">
+    <row r="348" spans="1:29" hidden="1">
       <c r="A348" s="14"/>
       <c r="D348" s="8" t="s">
         <v>107</v>
@@ -39670,7 +39702,7 @@
         <v>16F</v>
       </c>
     </row>
-    <row r="349" spans="1:29">
+    <row r="349" spans="1:29" hidden="1">
       <c r="A349" s="14"/>
       <c r="D349" s="8" t="s">
         <v>108</v>
@@ -39770,7 +39802,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="350" spans="1:29">
+    <row r="350" spans="1:29" hidden="1">
       <c r="A350" s="14"/>
       <c r="D350" s="8" t="s">
         <v>109</v>
@@ -39870,7 +39902,7 @@
         <v>19D</v>
       </c>
     </row>
-    <row r="351" spans="1:29">
+    <row r="351" spans="1:29" hidden="1">
       <c r="D351" s="8"/>
       <c r="E351" s="4"/>
       <c r="F351" s="4"/>
@@ -39896,7 +39928,7 @@
       <c r="Z351" s="4"/>
       <c r="AA351" s="4"/>
     </row>
-    <row r="352" spans="1:29">
+    <row r="352" spans="1:29" hidden="1">
       <c r="D352" s="7"/>
       <c r="E352" s="2"/>
       <c r="F352" s="2"/>
@@ -39921,15 +39953,18 @@
       <c r="Y352" s="2"/>
       <c r="Z352" s="2"/>
     </row>
-    <row r="353" spans="1:29">
+    <row r="353" spans="1:29" hidden="1">
       <c r="I353" s="5"/>
     </row>
-    <row r="357" spans="1:29">
+    <row r="354" spans="1:29" hidden="1"/>
+    <row r="355" spans="1:29" hidden="1"/>
+    <row r="356" spans="1:29" hidden="1"/>
+    <row r="357" spans="1:29" hidden="1">
       <c r="A357" s="5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="358" spans="1:29">
+    <row r="358" spans="1:29" hidden="1">
       <c r="G358" s="34">
         <v>0</v>
       </c>
@@ -40022,7 +40057,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="359" spans="1:29">
+    <row r="359" spans="1:29" hidden="1">
       <c r="G359" s="34">
         <f>AC358+1</f>
         <v>23</v>
@@ -40116,7 +40151,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="360" spans="1:29">
+    <row r="360" spans="1:29" hidden="1">
       <c r="G360" s="34">
         <f t="shared" ref="G360:G375" si="95">AC359+1</f>
         <v>46</v>
@@ -40210,7 +40245,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="361" spans="1:29">
+    <row r="361" spans="1:29" hidden="1">
       <c r="G361" s="34">
         <f t="shared" si="95"/>
         <v>69</v>
@@ -40304,7 +40339,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="362" spans="1:29">
+    <row r="362" spans="1:29" hidden="1">
       <c r="G362" s="34">
         <f t="shared" si="95"/>
         <v>92</v>
@@ -40398,7 +40433,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="363" spans="1:29">
+    <row r="363" spans="1:29" hidden="1">
       <c r="G363" s="34">
         <f t="shared" si="95"/>
         <v>115</v>
@@ -40492,7 +40527,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="364" spans="1:29">
+    <row r="364" spans="1:29" hidden="1">
       <c r="G364" s="34">
         <f t="shared" si="95"/>
         <v>138</v>
@@ -40586,7 +40621,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="365" spans="1:29">
+    <row r="365" spans="1:29" hidden="1">
       <c r="G365" s="34">
         <f t="shared" si="95"/>
         <v>161</v>
@@ -40680,7 +40715,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="366" spans="1:29">
+    <row r="366" spans="1:29" hidden="1">
       <c r="G366" s="34">
         <f t="shared" si="95"/>
         <v>184</v>
@@ -40774,7 +40809,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="367" spans="1:29">
+    <row r="367" spans="1:29" hidden="1">
       <c r="G367" s="34">
         <f t="shared" si="95"/>
         <v>207</v>
@@ -40868,7 +40903,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="368" spans="1:29">
+    <row r="368" spans="1:29" hidden="1">
       <c r="G368" s="34">
         <f t="shared" si="95"/>
         <v>230</v>
@@ -40962,7 +40997,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="369" spans="7:29">
+    <row r="369" spans="7:29" hidden="1">
       <c r="G369" s="34">
         <f t="shared" si="95"/>
         <v>253</v>
@@ -41056,7 +41091,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="370" spans="7:29">
+    <row r="370" spans="7:29" hidden="1">
       <c r="G370" s="34">
         <f t="shared" si="95"/>
         <v>276</v>
@@ -41150,7 +41185,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="371" spans="7:29">
+    <row r="371" spans="7:29" hidden="1">
       <c r="G371" s="34">
         <f t="shared" si="95"/>
         <v>299</v>
@@ -41244,7 +41279,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="372" spans="7:29">
+    <row r="372" spans="7:29" hidden="1">
       <c r="G372" s="34">
         <f t="shared" si="95"/>
         <v>322</v>
@@ -41338,7 +41373,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="373" spans="7:29">
+    <row r="373" spans="7:29" hidden="1">
       <c r="G373" s="34">
         <f t="shared" si="95"/>
         <v>345</v>
@@ -41432,7 +41467,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="374" spans="7:29">
+    <row r="374" spans="7:29" hidden="1">
       <c r="G374" s="34">
         <f t="shared" si="95"/>
         <v>368</v>
@@ -41526,7 +41561,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="375" spans="7:29">
+    <row r="375" spans="7:29" hidden="1">
       <c r="G375" s="34">
         <f t="shared" si="95"/>
         <v>391</v>
@@ -41620,17 +41655,30 @@
         <v>413</v>
       </c>
     </row>
-    <row r="388" spans="1:38" ht="23.25">
+    <row r="376" spans="7:29" hidden="1"/>
+    <row r="377" spans="7:29" hidden="1"/>
+    <row r="378" spans="7:29" hidden="1"/>
+    <row r="379" spans="7:29" hidden="1"/>
+    <row r="380" spans="7:29" hidden="1"/>
+    <row r="381" spans="7:29" hidden="1"/>
+    <row r="382" spans="7:29" hidden="1"/>
+    <row r="383" spans="7:29" hidden="1"/>
+    <row r="384" spans="7:29" hidden="1"/>
+    <row r="385" spans="1:38" hidden="1"/>
+    <row r="386" spans="1:38" hidden="1"/>
+    <row r="387" spans="1:38" hidden="1"/>
+    <row r="388" spans="1:38" ht="23.25" hidden="1">
       <c r="A388" s="13" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="390" spans="1:38" ht="23.25">
+    <row r="389" spans="1:38" hidden="1"/>
+    <row r="390" spans="1:38" ht="23.25" hidden="1">
       <c r="A390" s="13" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="391" spans="1:38" ht="18.75">
+    <row r="391" spans="1:38" ht="18.75" hidden="1">
       <c r="A391" t="s">
         <v>206</v>
       </c>
@@ -41638,10 +41686,10 @@
         <v>204</v>
       </c>
     </row>
-    <row r="392" spans="1:38" ht="18.75">
+    <row r="392" spans="1:38" ht="18.75" hidden="1">
       <c r="L392" s="18"/>
     </row>
-    <row r="393" spans="1:38" ht="18.75">
+    <row r="393" spans="1:38" ht="18.75" hidden="1">
       <c r="A393" t="s">
         <v>221</v>
       </c>
@@ -41654,13 +41702,13 @@
       </c>
       <c r="L393" s="18"/>
     </row>
-    <row r="394" spans="1:38" ht="18.75">
+    <row r="394" spans="1:38" ht="18.75" hidden="1">
       <c r="L394" s="18"/>
     </row>
-    <row r="395" spans="1:38" ht="18.75">
+    <row r="395" spans="1:38" ht="18.75" hidden="1">
       <c r="L395" s="18"/>
     </row>
-    <row r="396" spans="1:38" ht="18.75">
+    <row r="396" spans="1:38" ht="18.75" hidden="1">
       <c r="E396" t="s">
         <v>228</v>
       </c>
@@ -41673,7 +41721,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="397" spans="1:38" ht="18.75">
+    <row r="397" spans="1:38" ht="18.75" hidden="1">
       <c r="E397" t="s">
         <v>230</v>
       </c>
@@ -41682,13 +41730,13 @@
       </c>
       <c r="L397" s="18"/>
     </row>
-    <row r="398" spans="1:38" ht="18.75">
+    <row r="398" spans="1:38" ht="18.75" hidden="1">
       <c r="F398" s="6" t="s">
         <v>82</v>
       </c>
       <c r="L398" s="18"/>
     </row>
-    <row r="399" spans="1:38" ht="15.75" thickBot="1">
+    <row r="399" spans="1:38" ht="15.75" hidden="1" thickBot="1">
       <c r="A399" s="5" t="s">
         <v>94</v>
       </c>
@@ -41792,7 +41840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="400" spans="1:38" ht="16.5" thickTop="1" thickBot="1">
+    <row r="400" spans="1:38" ht="16.5" hidden="1" thickTop="1" thickBot="1">
       <c r="D400" s="6" t="s">
         <v>112</v>
       </c>
@@ -41929,7 +41977,7 @@
         <v>1F</v>
       </c>
     </row>
-    <row r="401" spans="1:38" ht="15.75" thickTop="1">
+    <row r="401" spans="1:38" ht="15.75" hidden="1" thickTop="1">
       <c r="D401" s="32">
         <v>-3</v>
       </c>
@@ -42064,7 +42112,7 @@
         <v>3F</v>
       </c>
     </row>
-    <row r="402" spans="1:38">
+    <row r="402" spans="1:38" hidden="1">
       <c r="D402" s="32">
         <v>-2</v>
       </c>
@@ -42199,7 +42247,7 @@
         <v>5F</v>
       </c>
     </row>
-    <row r="403" spans="1:38">
+    <row r="403" spans="1:38" hidden="1">
       <c r="D403" s="32">
         <v>-1</v>
       </c>
@@ -42334,7 +42382,7 @@
         <v>7F</v>
       </c>
     </row>
-    <row r="404" spans="1:38">
+    <row r="404" spans="1:38" hidden="1">
       <c r="A404" t="s">
         <v>93</v>
       </c>
@@ -42474,7 +42522,7 @@
         <v>9F</v>
       </c>
     </row>
-    <row r="405" spans="1:38">
+    <row r="405" spans="1:38" hidden="1">
       <c r="A405" s="17" t="s">
         <v>83</v>
       </c>
@@ -42614,7 +42662,7 @@
         <v>BF</v>
       </c>
     </row>
-    <row r="406" spans="1:38">
+    <row r="406" spans="1:38" hidden="1">
       <c r="A406" s="17" t="s">
         <v>84</v>
       </c>
@@ -42754,7 +42802,7 @@
         <v>DF</v>
       </c>
     </row>
-    <row r="407" spans="1:38">
+    <row r="407" spans="1:38" hidden="1">
       <c r="A407" s="17" t="s">
         <v>85</v>
       </c>
@@ -42894,7 +42942,7 @@
         <v>FF</v>
       </c>
     </row>
-    <row r="408" spans="1:38">
+    <row r="408" spans="1:38" hidden="1">
       <c r="A408" s="17" t="s">
         <v>86</v>
       </c>
@@ -43034,7 +43082,7 @@
         <v>11F</v>
       </c>
     </row>
-    <row r="409" spans="1:38">
+    <row r="409" spans="1:38" hidden="1">
       <c r="A409" s="17" t="s">
         <v>87</v>
       </c>
@@ -43174,7 +43222,7 @@
         <v>13F</v>
       </c>
     </row>
-    <row r="410" spans="1:38">
+    <row r="410" spans="1:38" hidden="1">
       <c r="A410" s="14" t="s">
         <v>88</v>
       </c>
@@ -43314,7 +43362,7 @@
         <v>15F</v>
       </c>
     </row>
-    <row r="411" spans="1:38">
+    <row r="411" spans="1:38" hidden="1">
       <c r="A411" s="14" t="s">
         <v>89</v>
       </c>
@@ -43454,7 +43502,7 @@
         <v>17F</v>
       </c>
     </row>
-    <row r="412" spans="1:38">
+    <row r="412" spans="1:38" hidden="1">
       <c r="A412" s="14" t="s">
         <v>90</v>
       </c>
@@ -43594,7 +43642,7 @@
         <v>19F</v>
       </c>
     </row>
-    <row r="413" spans="1:38">
+    <row r="413" spans="1:38" hidden="1">
       <c r="A413" s="14" t="s">
         <v>91</v>
       </c>
@@ -43734,7 +43782,7 @@
         <v>1BF</v>
       </c>
     </row>
-    <row r="414" spans="1:38">
+    <row r="414" spans="1:38" hidden="1">
       <c r="A414" s="14" t="s">
         <v>92</v>
       </c>
@@ -43874,7 +43922,7 @@
         <v>1DF</v>
       </c>
     </row>
-    <row r="415" spans="1:38">
+    <row r="415" spans="1:38" hidden="1">
       <c r="A415" s="14"/>
       <c r="D415" s="8" t="s">
         <v>107</v>
@@ -44010,7 +44058,7 @@
         <v>1FF</v>
       </c>
     </row>
-    <row r="416" spans="1:38">
+    <row r="416" spans="1:38" hidden="1">
       <c r="A416" s="14"/>
       <c r="D416" s="8" t="s">
         <v>108</v>
@@ -44146,7 +44194,7 @@
         <v>21F</v>
       </c>
     </row>
-    <row r="417" spans="1:38">
+    <row r="417" spans="1:38" hidden="1">
       <c r="A417" s="14"/>
       <c r="D417" s="8" t="s">
         <v>109</v>
@@ -44282,7 +44330,7 @@
         <v>23F</v>
       </c>
     </row>
-    <row r="418" spans="1:38">
+    <row r="418" spans="1:38" hidden="1">
       <c r="A418" s="14"/>
       <c r="D418" s="8" t="s">
         <v>110</v>
@@ -44418,7 +44466,7 @@
         <v>25E</v>
       </c>
     </row>
-    <row r="419" spans="1:38">
+    <row r="419" spans="1:38" hidden="1">
       <c r="D419" s="7"/>
       <c r="E419" s="2"/>
       <c r="F419" s="2"/>
@@ -44443,15 +44491,19 @@
       <c r="Z419" s="2"/>
       <c r="AA419" s="2"/>
     </row>
-    <row r="420" spans="1:38">
+    <row r="420" spans="1:38" hidden="1">
       <c r="I420" s="5"/>
     </row>
-    <row r="425" spans="1:38">
+    <row r="421" spans="1:38" hidden="1"/>
+    <row r="422" spans="1:38" hidden="1"/>
+    <row r="423" spans="1:38" hidden="1"/>
+    <row r="424" spans="1:38" hidden="1"/>
+    <row r="425" spans="1:38" hidden="1">
       <c r="A425" s="5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="426" spans="1:38">
+    <row r="426" spans="1:38" hidden="1">
       <c r="G426" s="34">
         <v>0</v>
       </c>
@@ -44580,7 +44632,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="427" spans="1:38">
+    <row r="427" spans="1:38" hidden="1">
       <c r="G427" s="34">
         <f>AL426+1</f>
         <v>32</v>
@@ -44710,7 +44762,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="428" spans="1:38">
+    <row r="428" spans="1:38" hidden="1">
       <c r="G428" s="34">
         <f t="shared" ref="G428:G444" si="208">AL427+1</f>
         <v>64</v>
@@ -44840,7 +44892,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="429" spans="1:38">
+    <row r="429" spans="1:38" hidden="1">
       <c r="G429" s="34">
         <f t="shared" si="208"/>
         <v>96</v>
@@ -44970,7 +45022,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="430" spans="1:38">
+    <row r="430" spans="1:38" hidden="1">
       <c r="G430" s="34">
         <f t="shared" si="208"/>
         <v>128</v>
@@ -45100,7 +45152,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="431" spans="1:38">
+    <row r="431" spans="1:38" hidden="1">
       <c r="G431" s="34">
         <f t="shared" si="208"/>
         <v>160</v>
@@ -45230,7 +45282,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="432" spans="1:38">
+    <row r="432" spans="1:38" hidden="1">
       <c r="G432" s="34">
         <f t="shared" si="208"/>
         <v>192</v>
@@ -45360,7 +45412,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="433" spans="7:38">
+    <row r="433" spans="7:38" hidden="1">
       <c r="G433" s="34">
         <f t="shared" si="208"/>
         <v>224</v>
@@ -45490,7 +45542,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="434" spans="7:38">
+    <row r="434" spans="7:38" hidden="1">
       <c r="G434" s="34">
         <f t="shared" si="208"/>
         <v>256</v>
@@ -45620,7 +45672,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="435" spans="7:38">
+    <row r="435" spans="7:38" hidden="1">
       <c r="G435" s="34">
         <f t="shared" si="208"/>
         <v>288</v>
@@ -45750,7 +45802,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="436" spans="7:38">
+    <row r="436" spans="7:38" hidden="1">
       <c r="G436" s="34">
         <f t="shared" si="208"/>
         <v>320</v>
@@ -45880,7 +45932,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="437" spans="7:38">
+    <row r="437" spans="7:38" hidden="1">
       <c r="G437" s="34">
         <f t="shared" si="208"/>
         <v>352</v>
@@ -46010,7 +46062,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="438" spans="7:38">
+    <row r="438" spans="7:38" hidden="1">
       <c r="G438" s="34">
         <f t="shared" si="208"/>
         <v>384</v>
@@ -46140,7 +46192,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="439" spans="7:38">
+    <row r="439" spans="7:38" hidden="1">
       <c r="G439" s="34">
         <f t="shared" si="208"/>
         <v>416</v>
@@ -46270,7 +46322,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="440" spans="7:38">
+    <row r="440" spans="7:38" hidden="1">
       <c r="G440" s="34">
         <f t="shared" si="208"/>
         <v>448</v>
@@ -46400,7 +46452,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="441" spans="7:38">
+    <row r="441" spans="7:38" hidden="1">
       <c r="G441" s="34">
         <f t="shared" si="208"/>
         <v>480</v>
@@ -46530,7 +46582,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="442" spans="7:38">
+    <row r="442" spans="7:38" hidden="1">
       <c r="G442" s="34">
         <f t="shared" si="208"/>
         <v>512</v>
@@ -46660,7 +46712,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="443" spans="7:38">
+    <row r="443" spans="7:38" hidden="1">
       <c r="G443" s="34">
         <f t="shared" si="208"/>
         <v>544</v>
@@ -46790,7 +46842,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="444" spans="7:38">
+    <row r="444" spans="7:38" hidden="1">
       <c r="G444" s="34">
         <f t="shared" si="208"/>
         <v>576</v>
@@ -46920,9 +46972,58 @@
         <v>607</v>
       </c>
     </row>
+    <row r="445" spans="7:38" hidden="1"/>
+    <row r="446" spans="7:38" hidden="1"/>
+    <row r="447" spans="7:38" hidden="1"/>
+    <row r="448" spans="7:38" hidden="1"/>
+    <row r="449" hidden="1"/>
+    <row r="450" hidden="1"/>
+    <row r="451" hidden="1"/>
+    <row r="452" hidden="1"/>
+    <row r="453" hidden="1"/>
+    <row r="454" hidden="1"/>
+    <row r="455" hidden="1"/>
+    <row r="456" hidden="1"/>
+    <row r="457" hidden="1"/>
+    <row r="458" hidden="1"/>
+    <row r="459" hidden="1"/>
+    <row r="460" hidden="1"/>
+    <row r="461" hidden="1"/>
+    <row r="462" hidden="1"/>
+    <row r="463" hidden="1"/>
+    <row r="464" hidden="1"/>
+    <row r="465" hidden="1"/>
+    <row r="466" hidden="1"/>
+    <row r="467" hidden="1"/>
+    <row r="468" hidden="1"/>
+    <row r="469" hidden="1"/>
+    <row r="470" hidden="1"/>
+    <row r="471" hidden="1"/>
+    <row r="472" hidden="1"/>
+    <row r="473" hidden="1"/>
+    <row r="474" hidden="1"/>
+    <row r="475" hidden="1"/>
+    <row r="476" hidden="1"/>
+    <row r="477" hidden="1"/>
+    <row r="478" hidden="1"/>
+    <row r="479" hidden="1"/>
+    <row r="480" hidden="1"/>
+    <row r="481" hidden="1"/>
+    <row r="482" hidden="1"/>
+    <row r="483" hidden="1"/>
+    <row r="484" hidden="1"/>
+    <row r="485" hidden="1"/>
+    <row r="486" hidden="1"/>
+    <row r="487" hidden="1"/>
+    <row r="488" hidden="1"/>
+    <row r="489" hidden="1"/>
+    <row r="490" hidden="1"/>
+    <row r="491" hidden="1"/>
+    <row r="492" hidden="1"/>
+    <row r="493" hidden="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="13" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="16" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
DEV Update: added tables to TOD, ELS, PLS Charts v0.01.xlsx
</commit_message>
<xml_diff>
--- a/Map_Shapes/Map/() darkness/TOD, ELS, PLS Charts v0.01.xlsx
+++ b/Map_Shapes/Map/() darkness/TOD, ELS, PLS Charts v0.01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="8235" windowHeight="3720"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="8235" windowHeight="3720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TOD (Sunrise_Sunset) Stencils" sheetId="10" r:id="rId1"/>
@@ -1496,7 +1496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E93" authorId="0">
+    <comment ref="E95" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3860,7 +3860,7 @@
   </sheetPr>
   <dimension ref="A1:BP406"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="Z35" sqref="Z35"/>
     </sheetView>
   </sheetViews>
@@ -25020,8 +25020,8 @@
   </sheetPr>
   <dimension ref="A1:BS493"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15:U21"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I113" sqref="I113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29703,9 +29703,6 @@
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
-      <c r="E93" s="4">
-        <v>0</v>
-      </c>
       <c r="F93" s="4"/>
       <c r="G93" s="35" t="str">
         <f t="shared" ref="G93:AM93" si="13">DEC2HEX(G123)</f>
@@ -29870,10 +29867,6 @@
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="E94" s="4">
-        <f>E93+1</f>
-        <v>1</v>
-      </c>
       <c r="F94" s="4"/>
       <c r="G94" s="35" t="str">
         <f t="shared" ref="G94:AM94" si="14">DEC2HEX(G124)</f>
@@ -30039,140 +30032,139 @@
         <v>6</v>
       </c>
       <c r="E95" s="4">
-        <f t="shared" ref="E95:E103" si="15">E94+1</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F95" s="4"/>
       <c r="G95" s="35" t="str">
-        <f t="shared" ref="G95:AM95" si="16">DEC2HEX(G125)</f>
+        <f t="shared" ref="G95:AM95" si="15">DEC2HEX(G125)</f>
         <v>C6</v>
       </c>
       <c r="H95" s="35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>C7</v>
       </c>
       <c r="I95" s="53" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>C8</v>
       </c>
       <c r="J95" s="61" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>C9</v>
       </c>
       <c r="K95" s="35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>CA</v>
       </c>
       <c r="L95" s="35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>CB</v>
       </c>
       <c r="M95" s="51" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>CC</v>
       </c>
       <c r="N95" s="51" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>CD</v>
       </c>
       <c r="O95" s="51" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>CE</v>
       </c>
       <c r="P95" s="51" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>CF</v>
       </c>
       <c r="Q95" s="51" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>D0</v>
       </c>
       <c r="R95" s="62" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>D1</v>
       </c>
       <c r="S95" s="62" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>D2</v>
       </c>
       <c r="T95" s="62" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>D3</v>
       </c>
       <c r="U95" s="62" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>D4</v>
       </c>
       <c r="V95" s="62" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>D5</v>
       </c>
       <c r="W95" s="62" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>D6</v>
       </c>
       <c r="X95" s="62" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>D7</v>
       </c>
       <c r="Y95" s="51" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>D8</v>
       </c>
       <c r="Z95" s="51" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>D9</v>
       </c>
       <c r="AA95" s="51" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>DA</v>
       </c>
       <c r="AB95" s="51" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>DB</v>
       </c>
       <c r="AC95" s="51" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>DC</v>
       </c>
       <c r="AD95" s="35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>DD</v>
       </c>
       <c r="AE95" s="35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>DE</v>
       </c>
       <c r="AF95" s="63" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>DF</v>
       </c>
       <c r="AG95" s="35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>E0</v>
       </c>
       <c r="AH95" s="35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>E1</v>
       </c>
       <c r="AI95" s="35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>E2</v>
       </c>
       <c r="AJ95" s="35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>E3</v>
       </c>
       <c r="AK95" s="35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>E4</v>
       </c>
       <c r="AL95" s="35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>E5</v>
       </c>
       <c r="AM95" s="35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>E6</v>
       </c>
       <c r="AS95" s="53"/>
@@ -30207,140 +30199,140 @@
         <v>7</v>
       </c>
       <c r="E96" s="4">
-        <f t="shared" si="15"/>
-        <v>3</v>
+        <f>E95+1</f>
+        <v>1</v>
       </c>
       <c r="F96" s="4"/>
       <c r="G96" s="35" t="str">
-        <f t="shared" ref="G96:AM96" si="17">DEC2HEX(G126)</f>
+        <f t="shared" ref="G96:AM96" si="16">DEC2HEX(G126)</f>
         <v>E7</v>
       </c>
       <c r="H96" s="35" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>E8</v>
       </c>
       <c r="I96" s="53" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>E9</v>
       </c>
       <c r="J96" s="61" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>EA</v>
       </c>
       <c r="K96" s="35" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>EB</v>
       </c>
       <c r="L96" s="35" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>EC</v>
       </c>
       <c r="M96" s="51" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>ED</v>
       </c>
       <c r="N96" s="51" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>EE</v>
       </c>
       <c r="O96" s="51" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>EF</v>
       </c>
       <c r="P96" s="51" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>F0</v>
       </c>
       <c r="Q96" s="51" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>F1</v>
       </c>
       <c r="R96" s="65" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>F2</v>
       </c>
       <c r="S96" s="62" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>F3</v>
       </c>
       <c r="T96" s="66" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>F4</v>
       </c>
       <c r="U96" s="62" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>F5</v>
       </c>
       <c r="V96" s="66" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>F6</v>
       </c>
       <c r="W96" s="62" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>F7</v>
       </c>
       <c r="X96" s="65" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>F8</v>
       </c>
       <c r="Y96" s="51" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>F9</v>
       </c>
       <c r="Z96" s="51" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>FA</v>
       </c>
       <c r="AA96" s="51" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>FB</v>
       </c>
       <c r="AB96" s="51" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>FC</v>
       </c>
       <c r="AC96" s="51" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>FD</v>
       </c>
       <c r="AD96" s="35" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>FE</v>
       </c>
       <c r="AE96" s="35" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>FF</v>
       </c>
       <c r="AF96" s="63" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>100</v>
       </c>
       <c r="AG96" s="35" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>101</v>
       </c>
       <c r="AH96" s="35" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>102</v>
       </c>
       <c r="AI96" s="35" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>103</v>
       </c>
       <c r="AJ96" s="35" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>104</v>
       </c>
       <c r="AK96" s="35" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>105</v>
       </c>
       <c r="AL96" s="35" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>106</v>
       </c>
       <c r="AM96" s="35" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>107</v>
       </c>
       <c r="AS96" s="53"/>
@@ -30375,8 +30367,8 @@
         <v>8</v>
       </c>
       <c r="E97" s="4">
-        <f t="shared" si="15"/>
-        <v>4</v>
+        <f t="shared" ref="E97:E105" si="17">E96+1</f>
+        <v>2</v>
       </c>
       <c r="F97" s="4"/>
       <c r="G97" s="35" t="str">
@@ -30543,8 +30535,8 @@
         <v>9</v>
       </c>
       <c r="E98" s="4">
-        <f t="shared" si="15"/>
-        <v>5</v>
+        <f t="shared" si="17"/>
+        <v>3</v>
       </c>
       <c r="F98" s="4"/>
       <c r="G98" s="35" t="str">
@@ -30710,8 +30702,8 @@
         <v>106</v>
       </c>
       <c r="E99" s="4">
-        <f t="shared" si="15"/>
-        <v>6</v>
+        <f t="shared" si="17"/>
+        <v>4</v>
       </c>
       <c r="F99" s="4"/>
       <c r="G99" s="35" t="str">
@@ -30877,8 +30869,8 @@
         <v>107</v>
       </c>
       <c r="E100" s="4">
-        <f t="shared" si="15"/>
-        <v>7</v>
+        <f t="shared" si="17"/>
+        <v>5</v>
       </c>
       <c r="F100" s="4"/>
       <c r="G100" s="35" t="str">
@@ -31044,8 +31036,8 @@
         <v>108</v>
       </c>
       <c r="E101" s="4">
-        <f t="shared" si="15"/>
-        <v>8</v>
+        <f t="shared" si="17"/>
+        <v>6</v>
       </c>
       <c r="F101" s="4"/>
       <c r="G101" s="35" t="str">
@@ -31211,8 +31203,8 @@
         <v>109</v>
       </c>
       <c r="E102" s="4">
-        <f t="shared" si="15"/>
-        <v>9</v>
+        <f t="shared" si="17"/>
+        <v>7</v>
       </c>
       <c r="F102" s="4"/>
       <c r="G102" s="35" t="str">
@@ -31378,8 +31370,8 @@
         <v>110</v>
       </c>
       <c r="E103" s="4">
-        <f t="shared" si="15"/>
-        <v>10</v>
+        <f t="shared" si="17"/>
+        <v>8</v>
       </c>
       <c r="F103" s="4"/>
       <c r="G103" s="35" t="str">
@@ -31544,7 +31536,10 @@
       <c r="D104" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="E104" s="4"/>
+      <c r="E104" s="4">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
       <c r="F104" s="4"/>
       <c r="G104" s="35" t="str">
         <f t="shared" ref="G104:AM104" si="25">DEC2HEX(G134)</f>
@@ -31708,7 +31703,10 @@
       <c r="D105" s="16">
         <v>10</v>
       </c>
-      <c r="E105" s="4"/>
+      <c r="E105" s="4">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
       <c r="F105" s="4"/>
       <c r="G105" s="35" t="str">
         <f t="shared" ref="G105:AM105" si="26">DEC2HEX(G135)</f>

</xml_diff>

<commit_message>
DEV UPDATE: **Bugs**. new offscreen ELS algorithm written. When I switch the clock to night time the game hangs.
</commit_message>
<xml_diff>
--- a/Map_Shapes/Map/() darkness/TOD, ELS, PLS Charts v0.01.xlsx
+++ b/Map_Shapes/Map/() darkness/TOD, ELS, PLS Charts v0.01.xlsx
@@ -25020,8 +25020,8 @@
   </sheetPr>
   <dimension ref="A1:BS493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I113" sqref="I113"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95:XFD95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>